<commit_message>
added santosh choudhary ecommerce website iora mockups
</commit_message>
<xml_diff>
--- a/Nitesh/myMonie_like_loanRequestForms/b2c form.xlsx
+++ b/Nitesh/myMonie_like_loanRequestForms/b2c form.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="178">
   <si>
     <t>Customer_Personal Loan</t>
   </si>
@@ -425,12 +425,138 @@
   <si>
     <t>Why you need to brrrow?</t>
   </si>
+  <si>
+    <t>Car Loan - New Salaried</t>
+  </si>
+  <si>
+    <t>Car Loan - New Self-employed</t>
+  </si>
+  <si>
+    <t>Car Loan - Used Salaried</t>
+  </si>
+  <si>
+    <t>Car Loan - Used Self-employed</t>
+  </si>
+  <si>
+    <t>Two Wheeler Loan - New Salaried</t>
+  </si>
+  <si>
+    <t>Two Wheeler Loan - New Self-employed</t>
+  </si>
+  <si>
+    <t>Two Wheeler Loan - Used Salaried</t>
+  </si>
+  <si>
+    <t>Two Wheeler Loan - Used Self employed</t>
+  </si>
+  <si>
+    <t>Commercial Vehicle Loan - New Salaried</t>
+  </si>
+  <si>
+    <t>Commercial Vehicle Loan - New Self employed</t>
+  </si>
+  <si>
+    <t>Commercial Vehicle Loan - Used Salaried</t>
+  </si>
+  <si>
+    <t>Commercial Vehicle Loan - Used Self employed</t>
+  </si>
+  <si>
+    <t>Education Loan Salaried</t>
+  </si>
+  <si>
+    <t>Education Loan self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  New Home Ready To Move (New) Salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  New Home Ready To Move (New) Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  New Home Ready To Move (Resale) Salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  New Home Ready To Move (Resale) Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  New Commercial Ready To Move  Salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  New Commercial Ready To Move  Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  Commercial Ready To Move  (Resale) Salarid</t>
+  </si>
+  <si>
+    <t>Home Loan   Commercial Ready To Move (Resale)  Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  New Industrial Property Ready To Move  Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  New Industrial Property Ready To Move  salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  Industrial Property Ready To Move (Resale) Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  Industrial Property Ready To Move (Resale) Salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  Under Construction (Flat)  Self employed</t>
+  </si>
+  <si>
+    <t>Home Loan  Under Construction (Flat)  Salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  New Commercial Under Construction Salaried</t>
+  </si>
+  <si>
+    <t>Home Loan  New Commercial Under Construction Self employed</t>
+  </si>
+  <si>
+    <t>Loan Type</t>
+  </si>
+  <si>
+    <t>customer Fname</t>
+  </si>
+  <si>
+    <t>customer Lname</t>
+  </si>
+  <si>
+    <t>Mobil</t>
+  </si>
+  <si>
+    <t>Your desired Loan Amount</t>
+  </si>
+  <si>
+    <t>Years in Current Profession</t>
+  </si>
+  <si>
+    <t>gross Annual Income</t>
+  </si>
+  <si>
+    <t>Where do you currently reside?</t>
+  </si>
+  <si>
+    <t>Total EMI you pay currently ?</t>
+  </si>
+  <si>
+    <t>Residence type</t>
+  </si>
+  <si>
+    <t>How are you currently employed ? </t>
+  </si>
+  <si>
+    <t>office/Shop/Factory</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +584,18 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arimo"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arimo"/>
@@ -510,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,6 +681,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,7 +779,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -668,7 +813,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -844,26 +988,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1449"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="57" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="28.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="6"/>
+    <col min="12" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1613,7 +1757,7 @@
       <c r="L52" s="7"/>
     </row>
     <row r="53" spans="4:12">
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="13" t="s">
@@ -15917,29 +16061,4585 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C1:AA1463"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="57" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:27" ht="22.2" customHeight="1">
+      <c r="C1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+    </row>
+    <row r="2" spans="3:27">
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:27">
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="3:27">
+      <c r="C4" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="3:27">
+      <c r="C5" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="3:27">
+      <c r="C6" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="3:27">
+      <c r="C7" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="3:27">
+      <c r="C8" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="3:27">
+      <c r="C9" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="3:27">
+      <c r="C10" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="3:27">
+      <c r="C11" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="3:27">
+      <c r="C12" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27">
+      <c r="C13" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="3:27">
+      <c r="C14" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="3:27">
+      <c r="C15" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="3:27">
+      <c r="C16" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66"/>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68"/>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70"/>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71"/>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72"/>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73"/>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74"/>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75"/>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76"/>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77"/>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78"/>
+    </row>
+    <row r="79" spans="3:3">
+      <c r="C79"/>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80"/>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81"/>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82"/>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83"/>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84"/>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85"/>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86"/>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87"/>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88"/>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89"/>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="3:3">
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="3:3">
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="3:3">
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="3:3">
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="3:3">
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="3:3">
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="3:3">
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="3:3">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="3:3">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="3:3">
+      <c r="C108"/>
+    </row>
+    <row r="109" spans="3:3">
+      <c r="C109"/>
+    </row>
+    <row r="110" spans="3:3">
+      <c r="C110"/>
+    </row>
+    <row r="111" spans="3:3">
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="3:3">
+      <c r="C112"/>
+    </row>
+    <row r="113" spans="3:3">
+      <c r="C113"/>
+    </row>
+    <row r="114" spans="3:3">
+      <c r="C114"/>
+    </row>
+    <row r="115" spans="3:3">
+      <c r="C115"/>
+    </row>
+    <row r="116" spans="3:3">
+      <c r="C116"/>
+    </row>
+    <row r="117" spans="3:3">
+      <c r="C117"/>
+    </row>
+    <row r="118" spans="3:3">
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="3:3">
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="3:3">
+      <c r="C120"/>
+    </row>
+    <row r="121" spans="3:3">
+      <c r="C121"/>
+    </row>
+    <row r="122" spans="3:3">
+      <c r="C122"/>
+    </row>
+    <row r="123" spans="3:3">
+      <c r="C123"/>
+    </row>
+    <row r="124" spans="3:3">
+      <c r="C124"/>
+    </row>
+    <row r="125" spans="3:3">
+      <c r="C125"/>
+    </row>
+    <row r="126" spans="3:3">
+      <c r="C126"/>
+    </row>
+    <row r="127" spans="3:3">
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="3:3">
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="3:3">
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="3:3">
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="3:3">
+      <c r="C131"/>
+    </row>
+    <row r="132" spans="3:3">
+      <c r="C132"/>
+    </row>
+    <row r="133" spans="3:3">
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="3:3">
+      <c r="C134"/>
+    </row>
+    <row r="135" spans="3:3">
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="3:3">
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="3:3">
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="3:3">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="3:3">
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="3:3">
+      <c r="C140"/>
+    </row>
+    <row r="141" spans="3:3">
+      <c r="C141"/>
+    </row>
+    <row r="142" spans="3:3">
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="3:3">
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="3:3">
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="3:3">
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="3:3">
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="3:3">
+      <c r="C147"/>
+    </row>
+    <row r="148" spans="3:3">
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="3:3">
+      <c r="C149"/>
+    </row>
+    <row r="150" spans="3:3">
+      <c r="C150"/>
+    </row>
+    <row r="151" spans="3:3">
+      <c r="C151"/>
+    </row>
+    <row r="152" spans="3:3">
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="3:3">
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="3:3">
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="3:3">
+      <c r="C155"/>
+    </row>
+    <row r="156" spans="3:3">
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="3:3">
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="3:3">
+      <c r="C158"/>
+    </row>
+    <row r="159" spans="3:3">
+      <c r="C159"/>
+    </row>
+    <row r="160" spans="3:3">
+      <c r="C160"/>
+    </row>
+    <row r="161" spans="3:3">
+      <c r="C161"/>
+    </row>
+    <row r="162" spans="3:3">
+      <c r="C162"/>
+    </row>
+    <row r="163" spans="3:3">
+      <c r="C163"/>
+    </row>
+    <row r="164" spans="3:3">
+      <c r="C164"/>
+    </row>
+    <row r="165" spans="3:3">
+      <c r="C165"/>
+    </row>
+    <row r="166" spans="3:3">
+      <c r="C166"/>
+    </row>
+    <row r="167" spans="3:3">
+      <c r="C167"/>
+    </row>
+    <row r="168" spans="3:3">
+      <c r="C168"/>
+    </row>
+    <row r="169" spans="3:3">
+      <c r="C169"/>
+    </row>
+    <row r="170" spans="3:3">
+      <c r="C170"/>
+    </row>
+    <row r="171" spans="3:3">
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="3:3">
+      <c r="C172"/>
+    </row>
+    <row r="173" spans="3:3">
+      <c r="C173"/>
+    </row>
+    <row r="174" spans="3:3">
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="3:3">
+      <c r="C175"/>
+    </row>
+    <row r="176" spans="3:3">
+      <c r="C176"/>
+    </row>
+    <row r="177" spans="3:3">
+      <c r="C177"/>
+    </row>
+    <row r="178" spans="3:3">
+      <c r="C178"/>
+    </row>
+    <row r="179" spans="3:3">
+      <c r="C179"/>
+    </row>
+    <row r="180" spans="3:3">
+      <c r="C180"/>
+    </row>
+    <row r="181" spans="3:3">
+      <c r="C181"/>
+    </row>
+    <row r="182" spans="3:3">
+      <c r="C182"/>
+    </row>
+    <row r="183" spans="3:3">
+      <c r="C183"/>
+    </row>
+    <row r="184" spans="3:3">
+      <c r="C184"/>
+    </row>
+    <row r="185" spans="3:3">
+      <c r="C185"/>
+    </row>
+    <row r="186" spans="3:3">
+      <c r="C186"/>
+    </row>
+    <row r="187" spans="3:3">
+      <c r="C187"/>
+    </row>
+    <row r="188" spans="3:3">
+      <c r="C188"/>
+    </row>
+    <row r="189" spans="3:3">
+      <c r="C189"/>
+    </row>
+    <row r="190" spans="3:3">
+      <c r="C190"/>
+    </row>
+    <row r="191" spans="3:3">
+      <c r="C191"/>
+    </row>
+    <row r="192" spans="3:3">
+      <c r="C192"/>
+    </row>
+    <row r="193" spans="3:3">
+      <c r="C193"/>
+    </row>
+    <row r="194" spans="3:3">
+      <c r="C194"/>
+    </row>
+    <row r="195" spans="3:3">
+      <c r="C195"/>
+    </row>
+    <row r="196" spans="3:3">
+      <c r="C196"/>
+    </row>
+    <row r="197" spans="3:3">
+      <c r="C197"/>
+    </row>
+    <row r="198" spans="3:3">
+      <c r="C198"/>
+    </row>
+    <row r="199" spans="3:3">
+      <c r="C199"/>
+    </row>
+    <row r="200" spans="3:3">
+      <c r="C200"/>
+    </row>
+    <row r="201" spans="3:3">
+      <c r="C201"/>
+    </row>
+    <row r="202" spans="3:3">
+      <c r="C202"/>
+    </row>
+    <row r="203" spans="3:3">
+      <c r="C203"/>
+    </row>
+    <row r="204" spans="3:3">
+      <c r="C204"/>
+    </row>
+    <row r="205" spans="3:3">
+      <c r="C205"/>
+    </row>
+    <row r="206" spans="3:3">
+      <c r="C206"/>
+    </row>
+    <row r="207" spans="3:3">
+      <c r="C207"/>
+    </row>
+    <row r="208" spans="3:3">
+      <c r="C208"/>
+    </row>
+    <row r="209" spans="3:3">
+      <c r="C209"/>
+    </row>
+    <row r="210" spans="3:3">
+      <c r="C210"/>
+    </row>
+    <row r="211" spans="3:3">
+      <c r="C211"/>
+    </row>
+    <row r="212" spans="3:3">
+      <c r="C212"/>
+    </row>
+    <row r="213" spans="3:3">
+      <c r="C213"/>
+    </row>
+    <row r="214" spans="3:3">
+      <c r="C214"/>
+    </row>
+    <row r="215" spans="3:3">
+      <c r="C215"/>
+    </row>
+    <row r="216" spans="3:3">
+      <c r="C216"/>
+    </row>
+    <row r="217" spans="3:3">
+      <c r="C217"/>
+    </row>
+    <row r="218" spans="3:3">
+      <c r="C218"/>
+    </row>
+    <row r="219" spans="3:3">
+      <c r="C219"/>
+    </row>
+    <row r="220" spans="3:3">
+      <c r="C220"/>
+    </row>
+    <row r="221" spans="3:3">
+      <c r="C221"/>
+    </row>
+    <row r="222" spans="3:3">
+      <c r="C222"/>
+    </row>
+    <row r="223" spans="3:3">
+      <c r="C223"/>
+    </row>
+    <row r="224" spans="3:3">
+      <c r="C224"/>
+    </row>
+    <row r="225" spans="3:3">
+      <c r="C225"/>
+    </row>
+    <row r="226" spans="3:3">
+      <c r="C226"/>
+    </row>
+    <row r="227" spans="3:3">
+      <c r="C227"/>
+    </row>
+    <row r="228" spans="3:3">
+      <c r="C228"/>
+    </row>
+    <row r="229" spans="3:3">
+      <c r="C229"/>
+    </row>
+    <row r="230" spans="3:3">
+      <c r="C230"/>
+    </row>
+    <row r="231" spans="3:3">
+      <c r="C231"/>
+    </row>
+    <row r="232" spans="3:3">
+      <c r="C232"/>
+    </row>
+    <row r="233" spans="3:3">
+      <c r="C233"/>
+    </row>
+    <row r="234" spans="3:3">
+      <c r="C234"/>
+    </row>
+    <row r="235" spans="3:3">
+      <c r="C235"/>
+    </row>
+    <row r="236" spans="3:3">
+      <c r="C236"/>
+    </row>
+    <row r="237" spans="3:3">
+      <c r="C237"/>
+    </row>
+    <row r="238" spans="3:3">
+      <c r="C238"/>
+    </row>
+    <row r="239" spans="3:3">
+      <c r="C239"/>
+    </row>
+    <row r="240" spans="3:3">
+      <c r="C240"/>
+    </row>
+    <row r="241" spans="3:3">
+      <c r="C241"/>
+    </row>
+    <row r="242" spans="3:3">
+      <c r="C242"/>
+    </row>
+    <row r="243" spans="3:3">
+      <c r="C243"/>
+    </row>
+    <row r="244" spans="3:3">
+      <c r="C244"/>
+    </row>
+    <row r="245" spans="3:3">
+      <c r="C245"/>
+    </row>
+    <row r="246" spans="3:3">
+      <c r="C246"/>
+    </row>
+    <row r="247" spans="3:3">
+      <c r="C247"/>
+    </row>
+    <row r="248" spans="3:3">
+      <c r="C248"/>
+    </row>
+    <row r="249" spans="3:3">
+      <c r="C249"/>
+    </row>
+    <row r="250" spans="3:3">
+      <c r="C250"/>
+    </row>
+    <row r="251" spans="3:3">
+      <c r="C251"/>
+    </row>
+    <row r="252" spans="3:3">
+      <c r="C252"/>
+    </row>
+    <row r="253" spans="3:3">
+      <c r="C253"/>
+    </row>
+    <row r="254" spans="3:3">
+      <c r="C254"/>
+    </row>
+    <row r="255" spans="3:3">
+      <c r="C255"/>
+    </row>
+    <row r="256" spans="3:3">
+      <c r="C256"/>
+    </row>
+    <row r="257" spans="3:3">
+      <c r="C257"/>
+    </row>
+    <row r="258" spans="3:3">
+      <c r="C258"/>
+    </row>
+    <row r="259" spans="3:3">
+      <c r="C259"/>
+    </row>
+    <row r="260" spans="3:3">
+      <c r="C260"/>
+    </row>
+    <row r="261" spans="3:3">
+      <c r="C261"/>
+    </row>
+    <row r="262" spans="3:3">
+      <c r="C262"/>
+    </row>
+    <row r="263" spans="3:3">
+      <c r="C263"/>
+    </row>
+    <row r="264" spans="3:3">
+      <c r="C264"/>
+    </row>
+    <row r="265" spans="3:3">
+      <c r="C265"/>
+    </row>
+    <row r="266" spans="3:3">
+      <c r="C266"/>
+    </row>
+    <row r="267" spans="3:3">
+      <c r="C267"/>
+    </row>
+    <row r="268" spans="3:3">
+      <c r="C268"/>
+    </row>
+    <row r="269" spans="3:3">
+      <c r="C269"/>
+    </row>
+    <row r="270" spans="3:3">
+      <c r="C270"/>
+    </row>
+    <row r="271" spans="3:3">
+      <c r="C271"/>
+    </row>
+    <row r="272" spans="3:3">
+      <c r="C272"/>
+    </row>
+    <row r="273" spans="3:3">
+      <c r="C273"/>
+    </row>
+    <row r="274" spans="3:3">
+      <c r="C274"/>
+    </row>
+    <row r="275" spans="3:3">
+      <c r="C275"/>
+    </row>
+    <row r="276" spans="3:3">
+      <c r="C276"/>
+    </row>
+    <row r="277" spans="3:3">
+      <c r="C277"/>
+    </row>
+    <row r="278" spans="3:3">
+      <c r="C278"/>
+    </row>
+    <row r="279" spans="3:3">
+      <c r="C279"/>
+    </row>
+    <row r="280" spans="3:3">
+      <c r="C280"/>
+    </row>
+    <row r="281" spans="3:3">
+      <c r="C281"/>
+    </row>
+    <row r="282" spans="3:3">
+      <c r="C282"/>
+    </row>
+    <row r="283" spans="3:3">
+      <c r="C283"/>
+    </row>
+    <row r="284" spans="3:3">
+      <c r="C284"/>
+    </row>
+    <row r="285" spans="3:3">
+      <c r="C285"/>
+    </row>
+    <row r="286" spans="3:3">
+      <c r="C286"/>
+    </row>
+    <row r="287" spans="3:3">
+      <c r="C287"/>
+    </row>
+    <row r="288" spans="3:3">
+      <c r="C288"/>
+    </row>
+    <row r="289" spans="3:3">
+      <c r="C289"/>
+    </row>
+    <row r="290" spans="3:3">
+      <c r="C290"/>
+    </row>
+    <row r="291" spans="3:3">
+      <c r="C291"/>
+    </row>
+    <row r="292" spans="3:3">
+      <c r="C292"/>
+    </row>
+    <row r="293" spans="3:3">
+      <c r="C293"/>
+    </row>
+    <row r="294" spans="3:3">
+      <c r="C294"/>
+    </row>
+    <row r="295" spans="3:3">
+      <c r="C295"/>
+    </row>
+    <row r="296" spans="3:3">
+      <c r="C296"/>
+    </row>
+    <row r="297" spans="3:3">
+      <c r="C297"/>
+    </row>
+    <row r="298" spans="3:3">
+      <c r="C298"/>
+    </row>
+    <row r="299" spans="3:3">
+      <c r="C299"/>
+    </row>
+    <row r="300" spans="3:3">
+      <c r="C300"/>
+    </row>
+    <row r="301" spans="3:3">
+      <c r="C301"/>
+    </row>
+    <row r="302" spans="3:3">
+      <c r="C302"/>
+    </row>
+    <row r="303" spans="3:3">
+      <c r="C303"/>
+    </row>
+    <row r="304" spans="3:3">
+      <c r="C304"/>
+    </row>
+    <row r="305" spans="3:3">
+      <c r="C305"/>
+    </row>
+    <row r="306" spans="3:3">
+      <c r="C306"/>
+    </row>
+    <row r="307" spans="3:3">
+      <c r="C307"/>
+    </row>
+    <row r="308" spans="3:3">
+      <c r="C308"/>
+    </row>
+    <row r="309" spans="3:3">
+      <c r="C309"/>
+    </row>
+    <row r="310" spans="3:3">
+      <c r="C310"/>
+    </row>
+    <row r="311" spans="3:3">
+      <c r="C311"/>
+    </row>
+    <row r="312" spans="3:3">
+      <c r="C312"/>
+    </row>
+    <row r="313" spans="3:3">
+      <c r="C313"/>
+    </row>
+    <row r="314" spans="3:3">
+      <c r="C314"/>
+    </row>
+    <row r="315" spans="3:3">
+      <c r="C315"/>
+    </row>
+    <row r="316" spans="3:3">
+      <c r="C316"/>
+    </row>
+    <row r="317" spans="3:3">
+      <c r="C317"/>
+    </row>
+    <row r="318" spans="3:3">
+      <c r="C318"/>
+    </row>
+    <row r="319" spans="3:3">
+      <c r="C319"/>
+    </row>
+    <row r="320" spans="3:3">
+      <c r="C320"/>
+    </row>
+    <row r="321" spans="3:3">
+      <c r="C321"/>
+    </row>
+    <row r="322" spans="3:3">
+      <c r="C322"/>
+    </row>
+    <row r="323" spans="3:3">
+      <c r="C323"/>
+    </row>
+    <row r="324" spans="3:3">
+      <c r="C324"/>
+    </row>
+    <row r="325" spans="3:3">
+      <c r="C325"/>
+    </row>
+    <row r="326" spans="3:3">
+      <c r="C326"/>
+    </row>
+    <row r="327" spans="3:3">
+      <c r="C327"/>
+    </row>
+    <row r="328" spans="3:3">
+      <c r="C328"/>
+    </row>
+    <row r="329" spans="3:3">
+      <c r="C329"/>
+    </row>
+    <row r="330" spans="3:3">
+      <c r="C330"/>
+    </row>
+    <row r="331" spans="3:3">
+      <c r="C331"/>
+    </row>
+    <row r="332" spans="3:3">
+      <c r="C332"/>
+    </row>
+    <row r="333" spans="3:3">
+      <c r="C333"/>
+    </row>
+    <row r="334" spans="3:3">
+      <c r="C334"/>
+    </row>
+    <row r="335" spans="3:3">
+      <c r="C335"/>
+    </row>
+    <row r="336" spans="3:3">
+      <c r="C336"/>
+    </row>
+    <row r="337" spans="3:3">
+      <c r="C337"/>
+    </row>
+    <row r="338" spans="3:3">
+      <c r="C338"/>
+    </row>
+    <row r="339" spans="3:3">
+      <c r="C339"/>
+    </row>
+    <row r="340" spans="3:3">
+      <c r="C340"/>
+    </row>
+    <row r="341" spans="3:3">
+      <c r="C341"/>
+    </row>
+    <row r="342" spans="3:3">
+      <c r="C342"/>
+    </row>
+    <row r="343" spans="3:3">
+      <c r="C343"/>
+    </row>
+    <row r="344" spans="3:3">
+      <c r="C344"/>
+    </row>
+    <row r="345" spans="3:3">
+      <c r="C345"/>
+    </row>
+    <row r="346" spans="3:3">
+      <c r="C346"/>
+    </row>
+    <row r="347" spans="3:3">
+      <c r="C347"/>
+    </row>
+    <row r="348" spans="3:3">
+      <c r="C348"/>
+    </row>
+    <row r="349" spans="3:3">
+      <c r="C349"/>
+    </row>
+    <row r="350" spans="3:3">
+      <c r="C350"/>
+    </row>
+    <row r="351" spans="3:3">
+      <c r="C351"/>
+    </row>
+    <row r="352" spans="3:3">
+      <c r="C352"/>
+    </row>
+    <row r="353" spans="3:3">
+      <c r="C353"/>
+    </row>
+    <row r="354" spans="3:3">
+      <c r="C354"/>
+    </row>
+    <row r="355" spans="3:3">
+      <c r="C355"/>
+    </row>
+    <row r="356" spans="3:3">
+      <c r="C356"/>
+    </row>
+    <row r="357" spans="3:3">
+      <c r="C357"/>
+    </row>
+    <row r="358" spans="3:3">
+      <c r="C358"/>
+    </row>
+    <row r="359" spans="3:3">
+      <c r="C359"/>
+    </row>
+    <row r="360" spans="3:3">
+      <c r="C360"/>
+    </row>
+    <row r="361" spans="3:3">
+      <c r="C361"/>
+    </row>
+    <row r="362" spans="3:3">
+      <c r="C362"/>
+    </row>
+    <row r="363" spans="3:3">
+      <c r="C363"/>
+    </row>
+    <row r="364" spans="3:3">
+      <c r="C364"/>
+    </row>
+    <row r="365" spans="3:3">
+      <c r="C365"/>
+    </row>
+    <row r="366" spans="3:3">
+      <c r="C366"/>
+    </row>
+    <row r="367" spans="3:3">
+      <c r="C367"/>
+    </row>
+    <row r="368" spans="3:3">
+      <c r="C368"/>
+    </row>
+    <row r="369" spans="3:3">
+      <c r="C369"/>
+    </row>
+    <row r="370" spans="3:3">
+      <c r="C370"/>
+    </row>
+    <row r="371" spans="3:3">
+      <c r="C371"/>
+    </row>
+    <row r="372" spans="3:3">
+      <c r="C372"/>
+    </row>
+    <row r="373" spans="3:3">
+      <c r="C373"/>
+    </row>
+    <row r="374" spans="3:3">
+      <c r="C374"/>
+    </row>
+    <row r="375" spans="3:3">
+      <c r="C375"/>
+    </row>
+    <row r="376" spans="3:3">
+      <c r="C376"/>
+    </row>
+    <row r="377" spans="3:3">
+      <c r="C377"/>
+    </row>
+    <row r="378" spans="3:3">
+      <c r="C378"/>
+    </row>
+    <row r="379" spans="3:3">
+      <c r="C379"/>
+    </row>
+    <row r="380" spans="3:3">
+      <c r="C380"/>
+    </row>
+    <row r="381" spans="3:3">
+      <c r="C381"/>
+    </row>
+    <row r="382" spans="3:3">
+      <c r="C382"/>
+    </row>
+    <row r="383" spans="3:3">
+      <c r="C383"/>
+    </row>
+    <row r="384" spans="3:3">
+      <c r="C384"/>
+    </row>
+    <row r="385" spans="3:3">
+      <c r="C385"/>
+    </row>
+    <row r="386" spans="3:3">
+      <c r="C386"/>
+    </row>
+    <row r="387" spans="3:3">
+      <c r="C387"/>
+    </row>
+    <row r="388" spans="3:3">
+      <c r="C388"/>
+    </row>
+    <row r="389" spans="3:3">
+      <c r="C389"/>
+    </row>
+    <row r="390" spans="3:3">
+      <c r="C390"/>
+    </row>
+    <row r="391" spans="3:3">
+      <c r="C391"/>
+    </row>
+    <row r="392" spans="3:3">
+      <c r="C392"/>
+    </row>
+    <row r="393" spans="3:3">
+      <c r="C393"/>
+    </row>
+    <row r="394" spans="3:3">
+      <c r="C394"/>
+    </row>
+    <row r="395" spans="3:3">
+      <c r="C395"/>
+    </row>
+    <row r="396" spans="3:3">
+      <c r="C396"/>
+    </row>
+    <row r="397" spans="3:3">
+      <c r="C397"/>
+    </row>
+    <row r="398" spans="3:3">
+      <c r="C398"/>
+    </row>
+    <row r="399" spans="3:3">
+      <c r="C399"/>
+    </row>
+    <row r="400" spans="3:3">
+      <c r="C400"/>
+    </row>
+    <row r="401" spans="3:3">
+      <c r="C401"/>
+    </row>
+    <row r="402" spans="3:3">
+      <c r="C402"/>
+    </row>
+    <row r="403" spans="3:3">
+      <c r="C403"/>
+    </row>
+    <row r="404" spans="3:3">
+      <c r="C404"/>
+    </row>
+    <row r="405" spans="3:3">
+      <c r="C405"/>
+    </row>
+    <row r="406" spans="3:3">
+      <c r="C406"/>
+    </row>
+    <row r="407" spans="3:3">
+      <c r="C407"/>
+    </row>
+    <row r="408" spans="3:3">
+      <c r="C408"/>
+    </row>
+    <row r="409" spans="3:3">
+      <c r="C409"/>
+    </row>
+    <row r="410" spans="3:3">
+      <c r="C410"/>
+    </row>
+    <row r="411" spans="3:3">
+      <c r="C411"/>
+    </row>
+    <row r="412" spans="3:3">
+      <c r="C412"/>
+    </row>
+    <row r="413" spans="3:3">
+      <c r="C413"/>
+    </row>
+    <row r="414" spans="3:3">
+      <c r="C414"/>
+    </row>
+    <row r="415" spans="3:3">
+      <c r="C415"/>
+    </row>
+    <row r="416" spans="3:3">
+      <c r="C416"/>
+    </row>
+    <row r="417" spans="3:3">
+      <c r="C417"/>
+    </row>
+    <row r="418" spans="3:3">
+      <c r="C418"/>
+    </row>
+    <row r="419" spans="3:3">
+      <c r="C419"/>
+    </row>
+    <row r="420" spans="3:3">
+      <c r="C420"/>
+    </row>
+    <row r="421" spans="3:3">
+      <c r="C421"/>
+    </row>
+    <row r="422" spans="3:3">
+      <c r="C422"/>
+    </row>
+    <row r="423" spans="3:3">
+      <c r="C423"/>
+    </row>
+    <row r="424" spans="3:3">
+      <c r="C424"/>
+    </row>
+    <row r="425" spans="3:3">
+      <c r="C425"/>
+    </row>
+    <row r="426" spans="3:3">
+      <c r="C426"/>
+    </row>
+    <row r="427" spans="3:3">
+      <c r="C427"/>
+    </row>
+    <row r="428" spans="3:3">
+      <c r="C428"/>
+    </row>
+    <row r="429" spans="3:3">
+      <c r="C429"/>
+    </row>
+    <row r="430" spans="3:3">
+      <c r="C430"/>
+    </row>
+    <row r="431" spans="3:3">
+      <c r="C431"/>
+    </row>
+    <row r="432" spans="3:3">
+      <c r="C432"/>
+    </row>
+    <row r="433" spans="3:3">
+      <c r="C433"/>
+    </row>
+    <row r="434" spans="3:3">
+      <c r="C434"/>
+    </row>
+    <row r="435" spans="3:3">
+      <c r="C435"/>
+    </row>
+    <row r="436" spans="3:3">
+      <c r="C436"/>
+    </row>
+    <row r="437" spans="3:3">
+      <c r="C437"/>
+    </row>
+    <row r="438" spans="3:3">
+      <c r="C438"/>
+    </row>
+    <row r="439" spans="3:3">
+      <c r="C439"/>
+    </row>
+    <row r="440" spans="3:3">
+      <c r="C440"/>
+    </row>
+    <row r="441" spans="3:3">
+      <c r="C441"/>
+    </row>
+    <row r="442" spans="3:3">
+      <c r="C442"/>
+    </row>
+    <row r="443" spans="3:3">
+      <c r="C443"/>
+    </row>
+    <row r="444" spans="3:3">
+      <c r="C444"/>
+    </row>
+    <row r="445" spans="3:3">
+      <c r="C445"/>
+    </row>
+    <row r="446" spans="3:3">
+      <c r="C446"/>
+    </row>
+    <row r="447" spans="3:3">
+      <c r="C447"/>
+    </row>
+    <row r="448" spans="3:3">
+      <c r="C448"/>
+    </row>
+    <row r="449" spans="3:3">
+      <c r="C449"/>
+    </row>
+    <row r="450" spans="3:3">
+      <c r="C450"/>
+    </row>
+    <row r="451" spans="3:3">
+      <c r="C451"/>
+    </row>
+    <row r="452" spans="3:3">
+      <c r="C452"/>
+    </row>
+    <row r="453" spans="3:3">
+      <c r="C453"/>
+    </row>
+    <row r="454" spans="3:3">
+      <c r="C454"/>
+    </row>
+    <row r="455" spans="3:3">
+      <c r="C455"/>
+    </row>
+    <row r="456" spans="3:3">
+      <c r="C456"/>
+    </row>
+    <row r="457" spans="3:3">
+      <c r="C457"/>
+    </row>
+    <row r="458" spans="3:3">
+      <c r="C458"/>
+    </row>
+    <row r="459" spans="3:3">
+      <c r="C459"/>
+    </row>
+    <row r="460" spans="3:3">
+      <c r="C460"/>
+    </row>
+    <row r="461" spans="3:3">
+      <c r="C461"/>
+    </row>
+    <row r="462" spans="3:3">
+      <c r="C462"/>
+    </row>
+    <row r="463" spans="3:3">
+      <c r="C463"/>
+    </row>
+    <row r="464" spans="3:3">
+      <c r="C464"/>
+    </row>
+    <row r="465" spans="3:3">
+      <c r="C465"/>
+    </row>
+    <row r="466" spans="3:3">
+      <c r="C466"/>
+    </row>
+    <row r="467" spans="3:3">
+      <c r="C467"/>
+    </row>
+    <row r="468" spans="3:3">
+      <c r="C468"/>
+    </row>
+    <row r="469" spans="3:3">
+      <c r="C469"/>
+    </row>
+    <row r="470" spans="3:3">
+      <c r="C470"/>
+    </row>
+    <row r="471" spans="3:3">
+      <c r="C471"/>
+    </row>
+    <row r="472" spans="3:3">
+      <c r="C472"/>
+    </row>
+    <row r="473" spans="3:3">
+      <c r="C473"/>
+    </row>
+    <row r="474" spans="3:3">
+      <c r="C474"/>
+    </row>
+    <row r="475" spans="3:3">
+      <c r="C475"/>
+    </row>
+    <row r="476" spans="3:3">
+      <c r="C476"/>
+    </row>
+    <row r="477" spans="3:3">
+      <c r="C477"/>
+    </row>
+    <row r="478" spans="3:3">
+      <c r="C478"/>
+    </row>
+    <row r="479" spans="3:3">
+      <c r="C479"/>
+    </row>
+    <row r="480" spans="3:3">
+      <c r="C480"/>
+    </row>
+    <row r="481" spans="3:3">
+      <c r="C481"/>
+    </row>
+    <row r="482" spans="3:3">
+      <c r="C482"/>
+    </row>
+    <row r="483" spans="3:3">
+      <c r="C483"/>
+    </row>
+    <row r="484" spans="3:3">
+      <c r="C484"/>
+    </row>
+    <row r="485" spans="3:3">
+      <c r="C485"/>
+    </row>
+    <row r="486" spans="3:3">
+      <c r="C486"/>
+    </row>
+    <row r="487" spans="3:3">
+      <c r="C487"/>
+    </row>
+    <row r="488" spans="3:3">
+      <c r="C488"/>
+    </row>
+    <row r="489" spans="3:3">
+      <c r="C489"/>
+    </row>
+    <row r="490" spans="3:3">
+      <c r="C490"/>
+    </row>
+    <row r="491" spans="3:3">
+      <c r="C491"/>
+    </row>
+    <row r="492" spans="3:3">
+      <c r="C492"/>
+    </row>
+    <row r="493" spans="3:3">
+      <c r="C493"/>
+    </row>
+    <row r="494" spans="3:3">
+      <c r="C494"/>
+    </row>
+    <row r="495" spans="3:3">
+      <c r="C495"/>
+    </row>
+    <row r="496" spans="3:3">
+      <c r="C496"/>
+    </row>
+    <row r="497" spans="3:3">
+      <c r="C497"/>
+    </row>
+    <row r="498" spans="3:3">
+      <c r="C498"/>
+    </row>
+    <row r="499" spans="3:3">
+      <c r="C499"/>
+    </row>
+    <row r="500" spans="3:3">
+      <c r="C500"/>
+    </row>
+    <row r="501" spans="3:3">
+      <c r="C501"/>
+    </row>
+    <row r="502" spans="3:3">
+      <c r="C502"/>
+    </row>
+    <row r="503" spans="3:3">
+      <c r="C503"/>
+    </row>
+    <row r="504" spans="3:3">
+      <c r="C504"/>
+    </row>
+    <row r="505" spans="3:3">
+      <c r="C505"/>
+    </row>
+    <row r="506" spans="3:3">
+      <c r="C506"/>
+    </row>
+    <row r="507" spans="3:3">
+      <c r="C507"/>
+    </row>
+    <row r="508" spans="3:3">
+      <c r="C508"/>
+    </row>
+    <row r="509" spans="3:3">
+      <c r="C509"/>
+    </row>
+    <row r="510" spans="3:3">
+      <c r="C510"/>
+    </row>
+    <row r="511" spans="3:3">
+      <c r="C511"/>
+    </row>
+    <row r="512" spans="3:3">
+      <c r="C512"/>
+    </row>
+    <row r="513" spans="3:3">
+      <c r="C513"/>
+    </row>
+    <row r="514" spans="3:3">
+      <c r="C514"/>
+    </row>
+    <row r="515" spans="3:3">
+      <c r="C515"/>
+    </row>
+    <row r="516" spans="3:3">
+      <c r="C516"/>
+    </row>
+    <row r="517" spans="3:3">
+      <c r="C517"/>
+    </row>
+    <row r="518" spans="3:3">
+      <c r="C518"/>
+    </row>
+    <row r="519" spans="3:3">
+      <c r="C519"/>
+    </row>
+    <row r="520" spans="3:3">
+      <c r="C520"/>
+    </row>
+    <row r="521" spans="3:3">
+      <c r="C521"/>
+    </row>
+    <row r="522" spans="3:3">
+      <c r="C522"/>
+    </row>
+    <row r="523" spans="3:3">
+      <c r="C523"/>
+    </row>
+    <row r="524" spans="3:3">
+      <c r="C524"/>
+    </row>
+    <row r="525" spans="3:3">
+      <c r="C525"/>
+    </row>
+    <row r="526" spans="3:3">
+      <c r="C526"/>
+    </row>
+    <row r="527" spans="3:3">
+      <c r="C527"/>
+    </row>
+    <row r="528" spans="3:3">
+      <c r="C528"/>
+    </row>
+    <row r="529" spans="3:3">
+      <c r="C529"/>
+    </row>
+    <row r="530" spans="3:3">
+      <c r="C530"/>
+    </row>
+    <row r="531" spans="3:3">
+      <c r="C531"/>
+    </row>
+    <row r="532" spans="3:3">
+      <c r="C532"/>
+    </row>
+    <row r="533" spans="3:3">
+      <c r="C533"/>
+    </row>
+    <row r="534" spans="3:3">
+      <c r="C534"/>
+    </row>
+    <row r="535" spans="3:3">
+      <c r="C535"/>
+    </row>
+    <row r="536" spans="3:3">
+      <c r="C536"/>
+    </row>
+    <row r="537" spans="3:3">
+      <c r="C537"/>
+    </row>
+    <row r="538" spans="3:3">
+      <c r="C538"/>
+    </row>
+    <row r="539" spans="3:3">
+      <c r="C539"/>
+    </row>
+    <row r="540" spans="3:3">
+      <c r="C540"/>
+    </row>
+    <row r="541" spans="3:3">
+      <c r="C541"/>
+    </row>
+    <row r="542" spans="3:3">
+      <c r="C542"/>
+    </row>
+    <row r="543" spans="3:3">
+      <c r="C543"/>
+    </row>
+    <row r="544" spans="3:3">
+      <c r="C544"/>
+    </row>
+    <row r="545" spans="3:3">
+      <c r="C545"/>
+    </row>
+    <row r="546" spans="3:3">
+      <c r="C546"/>
+    </row>
+    <row r="547" spans="3:3">
+      <c r="C547"/>
+    </row>
+    <row r="548" spans="3:3">
+      <c r="C548"/>
+    </row>
+    <row r="549" spans="3:3">
+      <c r="C549"/>
+    </row>
+    <row r="550" spans="3:3">
+      <c r="C550"/>
+    </row>
+    <row r="551" spans="3:3">
+      <c r="C551"/>
+    </row>
+    <row r="552" spans="3:3">
+      <c r="C552"/>
+    </row>
+    <row r="553" spans="3:3">
+      <c r="C553"/>
+    </row>
+    <row r="554" spans="3:3">
+      <c r="C554"/>
+    </row>
+    <row r="555" spans="3:3">
+      <c r="C555"/>
+    </row>
+    <row r="556" spans="3:3">
+      <c r="C556"/>
+    </row>
+    <row r="557" spans="3:3">
+      <c r="C557"/>
+    </row>
+    <row r="558" spans="3:3">
+      <c r="C558"/>
+    </row>
+    <row r="559" spans="3:3">
+      <c r="C559"/>
+    </row>
+    <row r="560" spans="3:3">
+      <c r="C560"/>
+    </row>
+    <row r="561" spans="3:3">
+      <c r="C561"/>
+    </row>
+    <row r="562" spans="3:3">
+      <c r="C562"/>
+    </row>
+    <row r="563" spans="3:3">
+      <c r="C563"/>
+    </row>
+    <row r="564" spans="3:3">
+      <c r="C564"/>
+    </row>
+    <row r="565" spans="3:3">
+      <c r="C565"/>
+    </row>
+    <row r="566" spans="3:3">
+      <c r="C566"/>
+    </row>
+    <row r="567" spans="3:3">
+      <c r="C567"/>
+    </row>
+    <row r="568" spans="3:3">
+      <c r="C568"/>
+    </row>
+    <row r="569" spans="3:3">
+      <c r="C569"/>
+    </row>
+    <row r="570" spans="3:3">
+      <c r="C570"/>
+    </row>
+    <row r="571" spans="3:3">
+      <c r="C571"/>
+    </row>
+    <row r="572" spans="3:3">
+      <c r="C572"/>
+    </row>
+    <row r="573" spans="3:3">
+      <c r="C573"/>
+    </row>
+    <row r="574" spans="3:3">
+      <c r="C574"/>
+    </row>
+    <row r="575" spans="3:3">
+      <c r="C575"/>
+    </row>
+    <row r="576" spans="3:3">
+      <c r="C576"/>
+    </row>
+    <row r="577" spans="3:3">
+      <c r="C577"/>
+    </row>
+    <row r="578" spans="3:3">
+      <c r="C578"/>
+    </row>
+    <row r="579" spans="3:3">
+      <c r="C579"/>
+    </row>
+    <row r="580" spans="3:3">
+      <c r="C580"/>
+    </row>
+    <row r="581" spans="3:3">
+      <c r="C581"/>
+    </row>
+    <row r="582" spans="3:3">
+      <c r="C582"/>
+    </row>
+    <row r="583" spans="3:3">
+      <c r="C583"/>
+    </row>
+    <row r="584" spans="3:3">
+      <c r="C584"/>
+    </row>
+    <row r="585" spans="3:3">
+      <c r="C585"/>
+    </row>
+    <row r="586" spans="3:3">
+      <c r="C586"/>
+    </row>
+    <row r="587" spans="3:3">
+      <c r="C587"/>
+    </row>
+    <row r="588" spans="3:3">
+      <c r="C588"/>
+    </row>
+    <row r="589" spans="3:3">
+      <c r="C589"/>
+    </row>
+    <row r="590" spans="3:3">
+      <c r="C590"/>
+    </row>
+    <row r="591" spans="3:3">
+      <c r="C591"/>
+    </row>
+    <row r="592" spans="3:3">
+      <c r="C592"/>
+    </row>
+    <row r="593" spans="3:3">
+      <c r="C593"/>
+    </row>
+    <row r="594" spans="3:3">
+      <c r="C594"/>
+    </row>
+    <row r="595" spans="3:3">
+      <c r="C595"/>
+    </row>
+    <row r="596" spans="3:3">
+      <c r="C596"/>
+    </row>
+    <row r="597" spans="3:3">
+      <c r="C597"/>
+    </row>
+    <row r="598" spans="3:3">
+      <c r="C598"/>
+    </row>
+    <row r="599" spans="3:3">
+      <c r="C599"/>
+    </row>
+    <row r="600" spans="3:3">
+      <c r="C600"/>
+    </row>
+    <row r="601" spans="3:3">
+      <c r="C601"/>
+    </row>
+    <row r="602" spans="3:3">
+      <c r="C602"/>
+    </row>
+    <row r="603" spans="3:3">
+      <c r="C603"/>
+    </row>
+    <row r="604" spans="3:3">
+      <c r="C604"/>
+    </row>
+    <row r="605" spans="3:3">
+      <c r="C605"/>
+    </row>
+    <row r="606" spans="3:3">
+      <c r="C606"/>
+    </row>
+    <row r="607" spans="3:3">
+      <c r="C607"/>
+    </row>
+    <row r="608" spans="3:3">
+      <c r="C608"/>
+    </row>
+    <row r="609" spans="3:3">
+      <c r="C609"/>
+    </row>
+    <row r="610" spans="3:3">
+      <c r="C610"/>
+    </row>
+    <row r="611" spans="3:3">
+      <c r="C611"/>
+    </row>
+    <row r="612" spans="3:3">
+      <c r="C612"/>
+    </row>
+    <row r="613" spans="3:3">
+      <c r="C613"/>
+    </row>
+    <row r="614" spans="3:3">
+      <c r="C614"/>
+    </row>
+    <row r="615" spans="3:3">
+      <c r="C615"/>
+    </row>
+    <row r="616" spans="3:3">
+      <c r="C616"/>
+    </row>
+    <row r="617" spans="3:3">
+      <c r="C617"/>
+    </row>
+    <row r="618" spans="3:3">
+      <c r="C618"/>
+    </row>
+    <row r="619" spans="3:3">
+      <c r="C619"/>
+    </row>
+    <row r="620" spans="3:3">
+      <c r="C620"/>
+    </row>
+    <row r="621" spans="3:3">
+      <c r="C621"/>
+    </row>
+    <row r="622" spans="3:3">
+      <c r="C622"/>
+    </row>
+    <row r="623" spans="3:3">
+      <c r="C623"/>
+    </row>
+    <row r="624" spans="3:3">
+      <c r="C624"/>
+    </row>
+    <row r="625" spans="3:3">
+      <c r="C625"/>
+    </row>
+    <row r="626" spans="3:3">
+      <c r="C626"/>
+    </row>
+    <row r="627" spans="3:3">
+      <c r="C627"/>
+    </row>
+    <row r="628" spans="3:3">
+      <c r="C628"/>
+    </row>
+    <row r="629" spans="3:3">
+      <c r="C629"/>
+    </row>
+    <row r="630" spans="3:3">
+      <c r="C630"/>
+    </row>
+    <row r="631" spans="3:3">
+      <c r="C631"/>
+    </row>
+    <row r="632" spans="3:3">
+      <c r="C632"/>
+    </row>
+    <row r="633" spans="3:3">
+      <c r="C633"/>
+    </row>
+    <row r="634" spans="3:3">
+      <c r="C634"/>
+    </row>
+    <row r="635" spans="3:3">
+      <c r="C635"/>
+    </row>
+    <row r="636" spans="3:3">
+      <c r="C636"/>
+    </row>
+    <row r="637" spans="3:3">
+      <c r="C637"/>
+    </row>
+    <row r="638" spans="3:3">
+      <c r="C638"/>
+    </row>
+    <row r="639" spans="3:3">
+      <c r="C639"/>
+    </row>
+    <row r="640" spans="3:3">
+      <c r="C640"/>
+    </row>
+    <row r="641" spans="3:3">
+      <c r="C641"/>
+    </row>
+    <row r="642" spans="3:3">
+      <c r="C642"/>
+    </row>
+    <row r="643" spans="3:3">
+      <c r="C643"/>
+    </row>
+    <row r="644" spans="3:3">
+      <c r="C644"/>
+    </row>
+    <row r="645" spans="3:3">
+      <c r="C645"/>
+    </row>
+    <row r="646" spans="3:3">
+      <c r="C646"/>
+    </row>
+    <row r="647" spans="3:3">
+      <c r="C647"/>
+    </row>
+    <row r="648" spans="3:3">
+      <c r="C648"/>
+    </row>
+    <row r="649" spans="3:3">
+      <c r="C649"/>
+    </row>
+    <row r="650" spans="3:3">
+      <c r="C650"/>
+    </row>
+    <row r="651" spans="3:3">
+      <c r="C651"/>
+    </row>
+    <row r="652" spans="3:3">
+      <c r="C652"/>
+    </row>
+    <row r="653" spans="3:3">
+      <c r="C653"/>
+    </row>
+    <row r="654" spans="3:3">
+      <c r="C654"/>
+    </row>
+    <row r="655" spans="3:3">
+      <c r="C655"/>
+    </row>
+    <row r="656" spans="3:3">
+      <c r="C656"/>
+    </row>
+    <row r="657" spans="3:3">
+      <c r="C657"/>
+    </row>
+    <row r="658" spans="3:3">
+      <c r="C658"/>
+    </row>
+    <row r="659" spans="3:3">
+      <c r="C659"/>
+    </row>
+    <row r="660" spans="3:3">
+      <c r="C660"/>
+    </row>
+    <row r="661" spans="3:3">
+      <c r="C661"/>
+    </row>
+    <row r="662" spans="3:3">
+      <c r="C662"/>
+    </row>
+    <row r="663" spans="3:3">
+      <c r="C663"/>
+    </row>
+    <row r="664" spans="3:3">
+      <c r="C664"/>
+    </row>
+    <row r="665" spans="3:3">
+      <c r="C665"/>
+    </row>
+    <row r="666" spans="3:3">
+      <c r="C666"/>
+    </row>
+    <row r="667" spans="3:3">
+      <c r="C667"/>
+    </row>
+    <row r="668" spans="3:3">
+      <c r="C668"/>
+    </row>
+    <row r="669" spans="3:3">
+      <c r="C669"/>
+    </row>
+    <row r="670" spans="3:3">
+      <c r="C670"/>
+    </row>
+    <row r="671" spans="3:3">
+      <c r="C671"/>
+    </row>
+    <row r="672" spans="3:3">
+      <c r="C672"/>
+    </row>
+    <row r="673" spans="3:3">
+      <c r="C673"/>
+    </row>
+    <row r="674" spans="3:3">
+      <c r="C674"/>
+    </row>
+    <row r="675" spans="3:3">
+      <c r="C675"/>
+    </row>
+    <row r="676" spans="3:3">
+      <c r="C676"/>
+    </row>
+    <row r="677" spans="3:3">
+      <c r="C677"/>
+    </row>
+    <row r="678" spans="3:3">
+      <c r="C678"/>
+    </row>
+    <row r="679" spans="3:3">
+      <c r="C679"/>
+    </row>
+    <row r="680" spans="3:3">
+      <c r="C680"/>
+    </row>
+    <row r="681" spans="3:3">
+      <c r="C681"/>
+    </row>
+    <row r="682" spans="3:3">
+      <c r="C682"/>
+    </row>
+    <row r="683" spans="3:3">
+      <c r="C683"/>
+    </row>
+    <row r="684" spans="3:3">
+      <c r="C684"/>
+    </row>
+    <row r="685" spans="3:3">
+      <c r="C685"/>
+    </row>
+    <row r="686" spans="3:3">
+      <c r="C686"/>
+    </row>
+    <row r="687" spans="3:3">
+      <c r="C687"/>
+    </row>
+    <row r="688" spans="3:3">
+      <c r="C688"/>
+    </row>
+    <row r="689" spans="3:3">
+      <c r="C689"/>
+    </row>
+    <row r="690" spans="3:3">
+      <c r="C690"/>
+    </row>
+    <row r="691" spans="3:3">
+      <c r="C691"/>
+    </row>
+    <row r="692" spans="3:3">
+      <c r="C692"/>
+    </row>
+    <row r="693" spans="3:3">
+      <c r="C693"/>
+    </row>
+    <row r="694" spans="3:3">
+      <c r="C694"/>
+    </row>
+    <row r="695" spans="3:3">
+      <c r="C695"/>
+    </row>
+    <row r="696" spans="3:3">
+      <c r="C696"/>
+    </row>
+    <row r="697" spans="3:3">
+      <c r="C697"/>
+    </row>
+    <row r="698" spans="3:3">
+      <c r="C698"/>
+    </row>
+    <row r="699" spans="3:3">
+      <c r="C699"/>
+    </row>
+    <row r="700" spans="3:3">
+      <c r="C700"/>
+    </row>
+    <row r="701" spans="3:3">
+      <c r="C701"/>
+    </row>
+    <row r="702" spans="3:3">
+      <c r="C702"/>
+    </row>
+    <row r="703" spans="3:3">
+      <c r="C703"/>
+    </row>
+    <row r="704" spans="3:3">
+      <c r="C704"/>
+    </row>
+    <row r="705" spans="3:3">
+      <c r="C705"/>
+    </row>
+    <row r="706" spans="3:3">
+      <c r="C706"/>
+    </row>
+    <row r="707" spans="3:3">
+      <c r="C707"/>
+    </row>
+    <row r="708" spans="3:3">
+      <c r="C708"/>
+    </row>
+    <row r="709" spans="3:3">
+      <c r="C709"/>
+    </row>
+    <row r="710" spans="3:3">
+      <c r="C710"/>
+    </row>
+    <row r="711" spans="3:3">
+      <c r="C711"/>
+    </row>
+    <row r="712" spans="3:3">
+      <c r="C712"/>
+    </row>
+    <row r="713" spans="3:3">
+      <c r="C713"/>
+    </row>
+    <row r="714" spans="3:3">
+      <c r="C714"/>
+    </row>
+    <row r="715" spans="3:3">
+      <c r="C715"/>
+    </row>
+    <row r="716" spans="3:3">
+      <c r="C716"/>
+    </row>
+    <row r="717" spans="3:3">
+      <c r="C717"/>
+    </row>
+    <row r="718" spans="3:3">
+      <c r="C718"/>
+    </row>
+    <row r="719" spans="3:3">
+      <c r="C719"/>
+    </row>
+    <row r="720" spans="3:3">
+      <c r="C720"/>
+    </row>
+    <row r="721" spans="3:3">
+      <c r="C721"/>
+    </row>
+    <row r="722" spans="3:3">
+      <c r="C722"/>
+    </row>
+    <row r="723" spans="3:3">
+      <c r="C723"/>
+    </row>
+    <row r="724" spans="3:3">
+      <c r="C724"/>
+    </row>
+    <row r="725" spans="3:3">
+      <c r="C725"/>
+    </row>
+    <row r="726" spans="3:3">
+      <c r="C726"/>
+    </row>
+    <row r="727" spans="3:3">
+      <c r="C727"/>
+    </row>
+    <row r="728" spans="3:3">
+      <c r="C728"/>
+    </row>
+    <row r="729" spans="3:3">
+      <c r="C729"/>
+    </row>
+    <row r="730" spans="3:3">
+      <c r="C730"/>
+    </row>
+    <row r="731" spans="3:3">
+      <c r="C731"/>
+    </row>
+    <row r="732" spans="3:3">
+      <c r="C732"/>
+    </row>
+    <row r="733" spans="3:3">
+      <c r="C733"/>
+    </row>
+    <row r="734" spans="3:3">
+      <c r="C734"/>
+    </row>
+    <row r="735" spans="3:3">
+      <c r="C735"/>
+    </row>
+    <row r="736" spans="3:3">
+      <c r="C736"/>
+    </row>
+    <row r="737" spans="3:3">
+      <c r="C737"/>
+    </row>
+    <row r="738" spans="3:3">
+      <c r="C738"/>
+    </row>
+    <row r="739" spans="3:3">
+      <c r="C739"/>
+    </row>
+    <row r="740" spans="3:3">
+      <c r="C740"/>
+    </row>
+    <row r="741" spans="3:3">
+      <c r="C741"/>
+    </row>
+    <row r="742" spans="3:3">
+      <c r="C742"/>
+    </row>
+    <row r="743" spans="3:3">
+      <c r="C743"/>
+    </row>
+    <row r="744" spans="3:3">
+      <c r="C744"/>
+    </row>
+    <row r="745" spans="3:3">
+      <c r="C745"/>
+    </row>
+    <row r="746" spans="3:3">
+      <c r="C746"/>
+    </row>
+    <row r="747" spans="3:3">
+      <c r="C747"/>
+    </row>
+    <row r="748" spans="3:3">
+      <c r="C748"/>
+    </row>
+    <row r="749" spans="3:3">
+      <c r="C749"/>
+    </row>
+    <row r="750" spans="3:3">
+      <c r="C750"/>
+    </row>
+    <row r="751" spans="3:3">
+      <c r="C751"/>
+    </row>
+    <row r="752" spans="3:3">
+      <c r="C752"/>
+    </row>
+    <row r="753" spans="3:3">
+      <c r="C753"/>
+    </row>
+    <row r="754" spans="3:3">
+      <c r="C754"/>
+    </row>
+    <row r="755" spans="3:3">
+      <c r="C755"/>
+    </row>
+    <row r="756" spans="3:3">
+      <c r="C756"/>
+    </row>
+    <row r="757" spans="3:3">
+      <c r="C757"/>
+    </row>
+    <row r="758" spans="3:3">
+      <c r="C758"/>
+    </row>
+    <row r="759" spans="3:3">
+      <c r="C759"/>
+    </row>
+    <row r="760" spans="3:3">
+      <c r="C760"/>
+    </row>
+    <row r="761" spans="3:3">
+      <c r="C761"/>
+    </row>
+    <row r="762" spans="3:3">
+      <c r="C762"/>
+    </row>
+    <row r="763" spans="3:3">
+      <c r="C763"/>
+    </row>
+    <row r="764" spans="3:3">
+      <c r="C764"/>
+    </row>
+    <row r="765" spans="3:3">
+      <c r="C765"/>
+    </row>
+    <row r="766" spans="3:3">
+      <c r="C766"/>
+    </row>
+    <row r="767" spans="3:3">
+      <c r="C767"/>
+    </row>
+    <row r="768" spans="3:3">
+      <c r="C768"/>
+    </row>
+    <row r="769" spans="3:3">
+      <c r="C769"/>
+    </row>
+    <row r="770" spans="3:3">
+      <c r="C770"/>
+    </row>
+    <row r="771" spans="3:3">
+      <c r="C771"/>
+    </row>
+    <row r="772" spans="3:3">
+      <c r="C772"/>
+    </row>
+    <row r="773" spans="3:3">
+      <c r="C773"/>
+    </row>
+    <row r="774" spans="3:3">
+      <c r="C774"/>
+    </row>
+    <row r="775" spans="3:3">
+      <c r="C775"/>
+    </row>
+    <row r="776" spans="3:3">
+      <c r="C776"/>
+    </row>
+    <row r="777" spans="3:3">
+      <c r="C777"/>
+    </row>
+    <row r="778" spans="3:3">
+      <c r="C778"/>
+    </row>
+    <row r="779" spans="3:3">
+      <c r="C779"/>
+    </row>
+    <row r="780" spans="3:3">
+      <c r="C780"/>
+    </row>
+    <row r="781" spans="3:3">
+      <c r="C781"/>
+    </row>
+    <row r="782" spans="3:3">
+      <c r="C782"/>
+    </row>
+    <row r="783" spans="3:3">
+      <c r="C783"/>
+    </row>
+    <row r="784" spans="3:3">
+      <c r="C784"/>
+    </row>
+    <row r="785" spans="3:3">
+      <c r="C785"/>
+    </row>
+    <row r="786" spans="3:3">
+      <c r="C786"/>
+    </row>
+    <row r="787" spans="3:3">
+      <c r="C787"/>
+    </row>
+    <row r="788" spans="3:3">
+      <c r="C788"/>
+    </row>
+    <row r="789" spans="3:3">
+      <c r="C789"/>
+    </row>
+    <row r="790" spans="3:3">
+      <c r="C790"/>
+    </row>
+    <row r="791" spans="3:3">
+      <c r="C791"/>
+    </row>
+    <row r="792" spans="3:3">
+      <c r="C792"/>
+    </row>
+    <row r="793" spans="3:3">
+      <c r="C793"/>
+    </row>
+    <row r="794" spans="3:3">
+      <c r="C794"/>
+    </row>
+    <row r="795" spans="3:3">
+      <c r="C795"/>
+    </row>
+    <row r="796" spans="3:3">
+      <c r="C796"/>
+    </row>
+    <row r="797" spans="3:3">
+      <c r="C797"/>
+    </row>
+    <row r="798" spans="3:3">
+      <c r="C798"/>
+    </row>
+    <row r="799" spans="3:3">
+      <c r="C799"/>
+    </row>
+    <row r="800" spans="3:3">
+      <c r="C800"/>
+    </row>
+    <row r="801" spans="3:3">
+      <c r="C801"/>
+    </row>
+    <row r="802" spans="3:3">
+      <c r="C802"/>
+    </row>
+    <row r="803" spans="3:3">
+      <c r="C803"/>
+    </row>
+    <row r="804" spans="3:3">
+      <c r="C804"/>
+    </row>
+    <row r="805" spans="3:3">
+      <c r="C805"/>
+    </row>
+    <row r="806" spans="3:3">
+      <c r="C806"/>
+    </row>
+    <row r="807" spans="3:3">
+      <c r="C807"/>
+    </row>
+    <row r="808" spans="3:3">
+      <c r="C808"/>
+    </row>
+    <row r="809" spans="3:3">
+      <c r="C809"/>
+    </row>
+    <row r="810" spans="3:3">
+      <c r="C810"/>
+    </row>
+    <row r="811" spans="3:3">
+      <c r="C811"/>
+    </row>
+    <row r="812" spans="3:3">
+      <c r="C812"/>
+    </row>
+    <row r="813" spans="3:3">
+      <c r="C813"/>
+    </row>
+    <row r="814" spans="3:3">
+      <c r="C814"/>
+    </row>
+    <row r="815" spans="3:3">
+      <c r="C815"/>
+    </row>
+    <row r="816" spans="3:3">
+      <c r="C816"/>
+    </row>
+    <row r="817" spans="3:3">
+      <c r="C817"/>
+    </row>
+    <row r="818" spans="3:3">
+      <c r="C818"/>
+    </row>
+    <row r="819" spans="3:3">
+      <c r="C819"/>
+    </row>
+    <row r="820" spans="3:3">
+      <c r="C820"/>
+    </row>
+    <row r="821" spans="3:3">
+      <c r="C821"/>
+    </row>
+    <row r="822" spans="3:3">
+      <c r="C822"/>
+    </row>
+    <row r="823" spans="3:3">
+      <c r="C823"/>
+    </row>
+    <row r="824" spans="3:3">
+      <c r="C824"/>
+    </row>
+    <row r="825" spans="3:3">
+      <c r="C825"/>
+    </row>
+    <row r="826" spans="3:3">
+      <c r="C826"/>
+    </row>
+    <row r="827" spans="3:3">
+      <c r="C827"/>
+    </row>
+    <row r="828" spans="3:3">
+      <c r="C828"/>
+    </row>
+    <row r="829" spans="3:3">
+      <c r="C829"/>
+    </row>
+    <row r="830" spans="3:3">
+      <c r="C830"/>
+    </row>
+    <row r="831" spans="3:3">
+      <c r="C831"/>
+    </row>
+    <row r="832" spans="3:3">
+      <c r="C832"/>
+    </row>
+    <row r="833" spans="3:3">
+      <c r="C833"/>
+    </row>
+    <row r="834" spans="3:3">
+      <c r="C834"/>
+    </row>
+    <row r="835" spans="3:3">
+      <c r="C835"/>
+    </row>
+    <row r="836" spans="3:3">
+      <c r="C836"/>
+    </row>
+    <row r="837" spans="3:3">
+      <c r="C837"/>
+    </row>
+    <row r="838" spans="3:3">
+      <c r="C838"/>
+    </row>
+    <row r="839" spans="3:3">
+      <c r="C839"/>
+    </row>
+    <row r="840" spans="3:3">
+      <c r="C840"/>
+    </row>
+    <row r="841" spans="3:3">
+      <c r="C841"/>
+    </row>
+    <row r="842" spans="3:3">
+      <c r="C842"/>
+    </row>
+    <row r="843" spans="3:3">
+      <c r="C843"/>
+    </row>
+    <row r="844" spans="3:3">
+      <c r="C844"/>
+    </row>
+    <row r="845" spans="3:3">
+      <c r="C845"/>
+    </row>
+    <row r="846" spans="3:3">
+      <c r="C846"/>
+    </row>
+    <row r="847" spans="3:3">
+      <c r="C847"/>
+    </row>
+    <row r="848" spans="3:3">
+      <c r="C848"/>
+    </row>
+    <row r="849" spans="3:3">
+      <c r="C849"/>
+    </row>
+    <row r="850" spans="3:3">
+      <c r="C850"/>
+    </row>
+    <row r="851" spans="3:3">
+      <c r="C851"/>
+    </row>
+    <row r="852" spans="3:3">
+      <c r="C852"/>
+    </row>
+    <row r="853" spans="3:3">
+      <c r="C853"/>
+    </row>
+    <row r="854" spans="3:3">
+      <c r="C854"/>
+    </row>
+    <row r="855" spans="3:3">
+      <c r="C855"/>
+    </row>
+    <row r="856" spans="3:3">
+      <c r="C856"/>
+    </row>
+    <row r="857" spans="3:3">
+      <c r="C857"/>
+    </row>
+    <row r="858" spans="3:3">
+      <c r="C858"/>
+    </row>
+    <row r="859" spans="3:3">
+      <c r="C859"/>
+    </row>
+    <row r="860" spans="3:3">
+      <c r="C860"/>
+    </row>
+    <row r="861" spans="3:3">
+      <c r="C861"/>
+    </row>
+    <row r="862" spans="3:3">
+      <c r="C862"/>
+    </row>
+    <row r="863" spans="3:3">
+      <c r="C863"/>
+    </row>
+    <row r="864" spans="3:3">
+      <c r="C864"/>
+    </row>
+    <row r="865" spans="3:3">
+      <c r="C865"/>
+    </row>
+    <row r="866" spans="3:3">
+      <c r="C866"/>
+    </row>
+    <row r="867" spans="3:3">
+      <c r="C867"/>
+    </row>
+    <row r="868" spans="3:3">
+      <c r="C868"/>
+    </row>
+    <row r="869" spans="3:3">
+      <c r="C869"/>
+    </row>
+    <row r="870" spans="3:3">
+      <c r="C870"/>
+    </row>
+    <row r="871" spans="3:3">
+      <c r="C871"/>
+    </row>
+    <row r="872" spans="3:3">
+      <c r="C872"/>
+    </row>
+    <row r="873" spans="3:3">
+      <c r="C873"/>
+    </row>
+    <row r="874" spans="3:3">
+      <c r="C874"/>
+    </row>
+    <row r="875" spans="3:3">
+      <c r="C875"/>
+    </row>
+    <row r="876" spans="3:3">
+      <c r="C876"/>
+    </row>
+    <row r="877" spans="3:3">
+      <c r="C877"/>
+    </row>
+    <row r="878" spans="3:3">
+      <c r="C878"/>
+    </row>
+    <row r="879" spans="3:3">
+      <c r="C879"/>
+    </row>
+    <row r="880" spans="3:3">
+      <c r="C880"/>
+    </row>
+    <row r="881" spans="3:3">
+      <c r="C881"/>
+    </row>
+    <row r="882" spans="3:3">
+      <c r="C882"/>
+    </row>
+    <row r="883" spans="3:3">
+      <c r="C883"/>
+    </row>
+    <row r="884" spans="3:3">
+      <c r="C884"/>
+    </row>
+    <row r="885" spans="3:3">
+      <c r="C885"/>
+    </row>
+    <row r="886" spans="3:3">
+      <c r="C886"/>
+    </row>
+    <row r="887" spans="3:3">
+      <c r="C887"/>
+    </row>
+    <row r="888" spans="3:3">
+      <c r="C888"/>
+    </row>
+    <row r="889" spans="3:3">
+      <c r="C889"/>
+    </row>
+    <row r="890" spans="3:3">
+      <c r="C890"/>
+    </row>
+    <row r="891" spans="3:3">
+      <c r="C891"/>
+    </row>
+    <row r="892" spans="3:3">
+      <c r="C892"/>
+    </row>
+    <row r="893" spans="3:3">
+      <c r="C893"/>
+    </row>
+    <row r="894" spans="3:3">
+      <c r="C894"/>
+    </row>
+    <row r="895" spans="3:3">
+      <c r="C895"/>
+    </row>
+    <row r="896" spans="3:3">
+      <c r="C896"/>
+    </row>
+    <row r="897" spans="3:3">
+      <c r="C897"/>
+    </row>
+    <row r="898" spans="3:3">
+      <c r="C898"/>
+    </row>
+    <row r="899" spans="3:3">
+      <c r="C899"/>
+    </row>
+    <row r="900" spans="3:3">
+      <c r="C900"/>
+    </row>
+    <row r="901" spans="3:3">
+      <c r="C901"/>
+    </row>
+    <row r="902" spans="3:3">
+      <c r="C902"/>
+    </row>
+    <row r="903" spans="3:3">
+      <c r="C903"/>
+    </row>
+    <row r="904" spans="3:3">
+      <c r="C904"/>
+    </row>
+    <row r="905" spans="3:3">
+      <c r="C905"/>
+    </row>
+    <row r="906" spans="3:3">
+      <c r="C906"/>
+    </row>
+    <row r="907" spans="3:3">
+      <c r="C907"/>
+    </row>
+    <row r="908" spans="3:3">
+      <c r="C908"/>
+    </row>
+    <row r="909" spans="3:3">
+      <c r="C909"/>
+    </row>
+    <row r="910" spans="3:3">
+      <c r="C910"/>
+    </row>
+    <row r="911" spans="3:3">
+      <c r="C911"/>
+    </row>
+    <row r="912" spans="3:3">
+      <c r="C912"/>
+    </row>
+    <row r="913" spans="3:3">
+      <c r="C913"/>
+    </row>
+    <row r="914" spans="3:3">
+      <c r="C914"/>
+    </row>
+    <row r="915" spans="3:3">
+      <c r="C915"/>
+    </row>
+    <row r="916" spans="3:3">
+      <c r="C916"/>
+    </row>
+    <row r="917" spans="3:3">
+      <c r="C917"/>
+    </row>
+    <row r="918" spans="3:3">
+      <c r="C918"/>
+    </row>
+    <row r="919" spans="3:3">
+      <c r="C919"/>
+    </row>
+    <row r="920" spans="3:3">
+      <c r="C920"/>
+    </row>
+    <row r="921" spans="3:3">
+      <c r="C921"/>
+    </row>
+    <row r="922" spans="3:3">
+      <c r="C922"/>
+    </row>
+    <row r="923" spans="3:3">
+      <c r="C923"/>
+    </row>
+    <row r="924" spans="3:3">
+      <c r="C924"/>
+    </row>
+    <row r="925" spans="3:3">
+      <c r="C925"/>
+    </row>
+    <row r="926" spans="3:3">
+      <c r="C926"/>
+    </row>
+    <row r="927" spans="3:3">
+      <c r="C927"/>
+    </row>
+    <row r="928" spans="3:3">
+      <c r="C928"/>
+    </row>
+    <row r="929" spans="3:3">
+      <c r="C929"/>
+    </row>
+    <row r="930" spans="3:3">
+      <c r="C930"/>
+    </row>
+    <row r="931" spans="3:3">
+      <c r="C931"/>
+    </row>
+    <row r="932" spans="3:3">
+      <c r="C932"/>
+    </row>
+    <row r="933" spans="3:3">
+      <c r="C933"/>
+    </row>
+    <row r="934" spans="3:3">
+      <c r="C934"/>
+    </row>
+    <row r="935" spans="3:3">
+      <c r="C935"/>
+    </row>
+    <row r="936" spans="3:3">
+      <c r="C936"/>
+    </row>
+    <row r="937" spans="3:3">
+      <c r="C937"/>
+    </row>
+    <row r="938" spans="3:3">
+      <c r="C938"/>
+    </row>
+    <row r="939" spans="3:3">
+      <c r="C939"/>
+    </row>
+    <row r="940" spans="3:3">
+      <c r="C940"/>
+    </row>
+    <row r="941" spans="3:3">
+      <c r="C941"/>
+    </row>
+    <row r="942" spans="3:3">
+      <c r="C942"/>
+    </row>
+    <row r="943" spans="3:3">
+      <c r="C943"/>
+    </row>
+    <row r="944" spans="3:3">
+      <c r="C944"/>
+    </row>
+    <row r="945" spans="3:3">
+      <c r="C945"/>
+    </row>
+    <row r="946" spans="3:3">
+      <c r="C946"/>
+    </row>
+    <row r="947" spans="3:3">
+      <c r="C947"/>
+    </row>
+    <row r="948" spans="3:3">
+      <c r="C948"/>
+    </row>
+    <row r="949" spans="3:3">
+      <c r="C949"/>
+    </row>
+    <row r="950" spans="3:3">
+      <c r="C950"/>
+    </row>
+    <row r="951" spans="3:3">
+      <c r="C951"/>
+    </row>
+    <row r="952" spans="3:3">
+      <c r="C952"/>
+    </row>
+    <row r="953" spans="3:3">
+      <c r="C953"/>
+    </row>
+    <row r="954" spans="3:3">
+      <c r="C954"/>
+    </row>
+    <row r="955" spans="3:3">
+      <c r="C955"/>
+    </row>
+    <row r="956" spans="3:3">
+      <c r="C956"/>
+    </row>
+    <row r="957" spans="3:3">
+      <c r="C957"/>
+    </row>
+    <row r="958" spans="3:3">
+      <c r="C958"/>
+    </row>
+    <row r="959" spans="3:3">
+      <c r="C959"/>
+    </row>
+    <row r="960" spans="3:3">
+      <c r="C960"/>
+    </row>
+    <row r="961" spans="3:3">
+      <c r="C961"/>
+    </row>
+    <row r="962" spans="3:3">
+      <c r="C962"/>
+    </row>
+    <row r="963" spans="3:3">
+      <c r="C963"/>
+    </row>
+    <row r="964" spans="3:3">
+      <c r="C964"/>
+    </row>
+    <row r="965" spans="3:3">
+      <c r="C965"/>
+    </row>
+    <row r="966" spans="3:3">
+      <c r="C966"/>
+    </row>
+    <row r="967" spans="3:3">
+      <c r="C967"/>
+    </row>
+    <row r="968" spans="3:3">
+      <c r="C968"/>
+    </row>
+    <row r="969" spans="3:3">
+      <c r="C969"/>
+    </row>
+    <row r="970" spans="3:3">
+      <c r="C970"/>
+    </row>
+    <row r="971" spans="3:3">
+      <c r="C971"/>
+    </row>
+    <row r="972" spans="3:3">
+      <c r="C972"/>
+    </row>
+    <row r="973" spans="3:3">
+      <c r="C973"/>
+    </row>
+    <row r="974" spans="3:3">
+      <c r="C974"/>
+    </row>
+    <row r="975" spans="3:3">
+      <c r="C975"/>
+    </row>
+    <row r="976" spans="3:3">
+      <c r="C976"/>
+    </row>
+    <row r="977" spans="3:3">
+      <c r="C977"/>
+    </row>
+    <row r="978" spans="3:3">
+      <c r="C978"/>
+    </row>
+    <row r="979" spans="3:3">
+      <c r="C979"/>
+    </row>
+    <row r="980" spans="3:3">
+      <c r="C980"/>
+    </row>
+    <row r="981" spans="3:3">
+      <c r="C981"/>
+    </row>
+    <row r="982" spans="3:3">
+      <c r="C982"/>
+    </row>
+    <row r="983" spans="3:3">
+      <c r="C983"/>
+    </row>
+    <row r="984" spans="3:3">
+      <c r="C984"/>
+    </row>
+    <row r="985" spans="3:3">
+      <c r="C985"/>
+    </row>
+    <row r="986" spans="3:3">
+      <c r="C986"/>
+    </row>
+    <row r="987" spans="3:3">
+      <c r="C987"/>
+    </row>
+    <row r="988" spans="3:3">
+      <c r="C988"/>
+    </row>
+    <row r="989" spans="3:3">
+      <c r="C989"/>
+    </row>
+    <row r="990" spans="3:3">
+      <c r="C990"/>
+    </row>
+    <row r="991" spans="3:3">
+      <c r="C991"/>
+    </row>
+    <row r="992" spans="3:3">
+      <c r="C992"/>
+    </row>
+    <row r="993" spans="3:3">
+      <c r="C993"/>
+    </row>
+    <row r="994" spans="3:3">
+      <c r="C994"/>
+    </row>
+    <row r="995" spans="3:3">
+      <c r="C995"/>
+    </row>
+    <row r="996" spans="3:3">
+      <c r="C996"/>
+    </row>
+    <row r="997" spans="3:3">
+      <c r="C997"/>
+    </row>
+    <row r="998" spans="3:3">
+      <c r="C998"/>
+    </row>
+    <row r="999" spans="3:3">
+      <c r="C999"/>
+    </row>
+    <row r="1000" spans="3:3">
+      <c r="C1000"/>
+    </row>
+    <row r="1001" spans="3:3">
+      <c r="C1001"/>
+    </row>
+    <row r="1002" spans="3:3">
+      <c r="C1002"/>
+    </row>
+    <row r="1003" spans="3:3">
+      <c r="C1003"/>
+    </row>
+    <row r="1004" spans="3:3">
+      <c r="C1004"/>
+    </row>
+    <row r="1005" spans="3:3">
+      <c r="C1005"/>
+    </row>
+    <row r="1006" spans="3:3">
+      <c r="C1006"/>
+    </row>
+    <row r="1007" spans="3:3">
+      <c r="C1007"/>
+    </row>
+    <row r="1008" spans="3:3">
+      <c r="C1008"/>
+    </row>
+    <row r="1009" spans="3:3">
+      <c r="C1009"/>
+    </row>
+    <row r="1010" spans="3:3">
+      <c r="C1010"/>
+    </row>
+    <row r="1011" spans="3:3">
+      <c r="C1011"/>
+    </row>
+    <row r="1012" spans="3:3">
+      <c r="C1012"/>
+    </row>
+    <row r="1013" spans="3:3">
+      <c r="C1013"/>
+    </row>
+    <row r="1014" spans="3:3">
+      <c r="C1014"/>
+    </row>
+    <row r="1015" spans="3:3">
+      <c r="C1015"/>
+    </row>
+    <row r="1016" spans="3:3">
+      <c r="C1016"/>
+    </row>
+    <row r="1017" spans="3:3">
+      <c r="C1017"/>
+    </row>
+    <row r="1018" spans="3:3">
+      <c r="C1018"/>
+    </row>
+    <row r="1019" spans="3:3">
+      <c r="C1019"/>
+    </row>
+    <row r="1020" spans="3:3">
+      <c r="C1020"/>
+    </row>
+    <row r="1021" spans="3:3">
+      <c r="C1021"/>
+    </row>
+    <row r="1022" spans="3:3">
+      <c r="C1022"/>
+    </row>
+    <row r="1023" spans="3:3">
+      <c r="C1023"/>
+    </row>
+    <row r="1024" spans="3:3">
+      <c r="C1024"/>
+    </row>
+    <row r="1025" spans="3:3">
+      <c r="C1025"/>
+    </row>
+    <row r="1026" spans="3:3">
+      <c r="C1026"/>
+    </row>
+    <row r="1027" spans="3:3">
+      <c r="C1027"/>
+    </row>
+    <row r="1028" spans="3:3">
+      <c r="C1028"/>
+    </row>
+    <row r="1029" spans="3:3">
+      <c r="C1029"/>
+    </row>
+    <row r="1030" spans="3:3">
+      <c r="C1030"/>
+    </row>
+    <row r="1031" spans="3:3">
+      <c r="C1031"/>
+    </row>
+    <row r="1032" spans="3:3">
+      <c r="C1032"/>
+    </row>
+    <row r="1033" spans="3:3">
+      <c r="C1033"/>
+    </row>
+    <row r="1034" spans="3:3">
+      <c r="C1034"/>
+    </row>
+    <row r="1035" spans="3:3">
+      <c r="C1035"/>
+    </row>
+    <row r="1036" spans="3:3">
+      <c r="C1036"/>
+    </row>
+    <row r="1037" spans="3:3">
+      <c r="C1037"/>
+    </row>
+    <row r="1038" spans="3:3">
+      <c r="C1038"/>
+    </row>
+    <row r="1039" spans="3:3">
+      <c r="C1039"/>
+    </row>
+    <row r="1040" spans="3:3">
+      <c r="C1040"/>
+    </row>
+    <row r="1041" spans="3:3">
+      <c r="C1041"/>
+    </row>
+    <row r="1042" spans="3:3">
+      <c r="C1042"/>
+    </row>
+    <row r="1043" spans="3:3">
+      <c r="C1043"/>
+    </row>
+    <row r="1044" spans="3:3">
+      <c r="C1044"/>
+    </row>
+    <row r="1045" spans="3:3">
+      <c r="C1045"/>
+    </row>
+    <row r="1046" spans="3:3">
+      <c r="C1046"/>
+    </row>
+    <row r="1047" spans="3:3">
+      <c r="C1047"/>
+    </row>
+    <row r="1048" spans="3:3">
+      <c r="C1048"/>
+    </row>
+    <row r="1049" spans="3:3">
+      <c r="C1049"/>
+    </row>
+    <row r="1050" spans="3:3">
+      <c r="C1050"/>
+    </row>
+    <row r="1051" spans="3:3">
+      <c r="C1051"/>
+    </row>
+    <row r="1052" spans="3:3">
+      <c r="C1052"/>
+    </row>
+    <row r="1053" spans="3:3">
+      <c r="C1053"/>
+    </row>
+    <row r="1054" spans="3:3">
+      <c r="C1054"/>
+    </row>
+    <row r="1055" spans="3:3">
+      <c r="C1055"/>
+    </row>
+    <row r="1056" spans="3:3">
+      <c r="C1056"/>
+    </row>
+    <row r="1057" spans="3:3">
+      <c r="C1057"/>
+    </row>
+    <row r="1058" spans="3:3">
+      <c r="C1058"/>
+    </row>
+    <row r="1059" spans="3:3">
+      <c r="C1059"/>
+    </row>
+    <row r="1060" spans="3:3">
+      <c r="C1060"/>
+    </row>
+    <row r="1061" spans="3:3">
+      <c r="C1061"/>
+    </row>
+    <row r="1062" spans="3:3">
+      <c r="C1062"/>
+    </row>
+    <row r="1063" spans="3:3">
+      <c r="C1063"/>
+    </row>
+    <row r="1064" spans="3:3">
+      <c r="C1064"/>
+    </row>
+    <row r="1065" spans="3:3">
+      <c r="C1065"/>
+    </row>
+    <row r="1066" spans="3:3">
+      <c r="C1066"/>
+    </row>
+    <row r="1067" spans="3:3">
+      <c r="C1067"/>
+    </row>
+    <row r="1068" spans="3:3">
+      <c r="C1068"/>
+    </row>
+    <row r="1069" spans="3:3">
+      <c r="C1069"/>
+    </row>
+    <row r="1070" spans="3:3">
+      <c r="C1070"/>
+    </row>
+    <row r="1071" spans="3:3">
+      <c r="C1071"/>
+    </row>
+    <row r="1072" spans="3:3">
+      <c r="C1072"/>
+    </row>
+    <row r="1073" spans="3:3">
+      <c r="C1073"/>
+    </row>
+    <row r="1074" spans="3:3">
+      <c r="C1074"/>
+    </row>
+    <row r="1075" spans="3:3">
+      <c r="C1075"/>
+    </row>
+    <row r="1076" spans="3:3">
+      <c r="C1076"/>
+    </row>
+    <row r="1077" spans="3:3">
+      <c r="C1077"/>
+    </row>
+    <row r="1078" spans="3:3">
+      <c r="C1078"/>
+    </row>
+    <row r="1079" spans="3:3">
+      <c r="C1079"/>
+    </row>
+    <row r="1080" spans="3:3">
+      <c r="C1080"/>
+    </row>
+    <row r="1081" spans="3:3">
+      <c r="C1081"/>
+    </row>
+    <row r="1082" spans="3:3">
+      <c r="C1082"/>
+    </row>
+    <row r="1083" spans="3:3">
+      <c r="C1083"/>
+    </row>
+    <row r="1084" spans="3:3">
+      <c r="C1084"/>
+    </row>
+    <row r="1085" spans="3:3">
+      <c r="C1085"/>
+    </row>
+    <row r="1086" spans="3:3">
+      <c r="C1086"/>
+    </row>
+    <row r="1087" spans="3:3">
+      <c r="C1087"/>
+    </row>
+    <row r="1088" spans="3:3">
+      <c r="C1088"/>
+    </row>
+    <row r="1089" spans="3:3">
+      <c r="C1089"/>
+    </row>
+    <row r="1090" spans="3:3">
+      <c r="C1090"/>
+    </row>
+    <row r="1091" spans="3:3">
+      <c r="C1091"/>
+    </row>
+    <row r="1092" spans="3:3">
+      <c r="C1092"/>
+    </row>
+    <row r="1093" spans="3:3">
+      <c r="C1093"/>
+    </row>
+    <row r="1094" spans="3:3">
+      <c r="C1094"/>
+    </row>
+    <row r="1095" spans="3:3">
+      <c r="C1095"/>
+    </row>
+    <row r="1096" spans="3:3">
+      <c r="C1096"/>
+    </row>
+    <row r="1097" spans="3:3">
+      <c r="C1097"/>
+    </row>
+    <row r="1098" spans="3:3">
+      <c r="C1098"/>
+    </row>
+    <row r="1099" spans="3:3">
+      <c r="C1099"/>
+    </row>
+    <row r="1100" spans="3:3">
+      <c r="C1100"/>
+    </row>
+    <row r="1101" spans="3:3">
+      <c r="C1101"/>
+    </row>
+    <row r="1102" spans="3:3">
+      <c r="C1102"/>
+    </row>
+    <row r="1103" spans="3:3">
+      <c r="C1103"/>
+    </row>
+    <row r="1104" spans="3:3">
+      <c r="C1104"/>
+    </row>
+    <row r="1105" spans="3:3">
+      <c r="C1105"/>
+    </row>
+    <row r="1106" spans="3:3">
+      <c r="C1106"/>
+    </row>
+    <row r="1107" spans="3:3">
+      <c r="C1107"/>
+    </row>
+    <row r="1108" spans="3:3">
+      <c r="C1108"/>
+    </row>
+    <row r="1109" spans="3:3">
+      <c r="C1109"/>
+    </row>
+    <row r="1110" spans="3:3">
+      <c r="C1110"/>
+    </row>
+    <row r="1111" spans="3:3">
+      <c r="C1111"/>
+    </row>
+    <row r="1112" spans="3:3">
+      <c r="C1112"/>
+    </row>
+    <row r="1113" spans="3:3">
+      <c r="C1113"/>
+    </row>
+    <row r="1114" spans="3:3">
+      <c r="C1114"/>
+    </row>
+    <row r="1115" spans="3:3">
+      <c r="C1115"/>
+    </row>
+    <row r="1116" spans="3:3">
+      <c r="C1116"/>
+    </row>
+    <row r="1117" spans="3:3">
+      <c r="C1117"/>
+    </row>
+    <row r="1118" spans="3:3">
+      <c r="C1118"/>
+    </row>
+    <row r="1119" spans="3:3">
+      <c r="C1119"/>
+    </row>
+    <row r="1120" spans="3:3">
+      <c r="C1120"/>
+    </row>
+    <row r="1121" spans="3:3">
+      <c r="C1121"/>
+    </row>
+    <row r="1122" spans="3:3">
+      <c r="C1122"/>
+    </row>
+    <row r="1123" spans="3:3">
+      <c r="C1123"/>
+    </row>
+    <row r="1124" spans="3:3">
+      <c r="C1124"/>
+    </row>
+    <row r="1125" spans="3:3">
+      <c r="C1125"/>
+    </row>
+    <row r="1126" spans="3:3">
+      <c r="C1126"/>
+    </row>
+    <row r="1127" spans="3:3">
+      <c r="C1127"/>
+    </row>
+    <row r="1128" spans="3:3">
+      <c r="C1128"/>
+    </row>
+    <row r="1129" spans="3:3">
+      <c r="C1129"/>
+    </row>
+    <row r="1130" spans="3:3">
+      <c r="C1130"/>
+    </row>
+    <row r="1131" spans="3:3">
+      <c r="C1131"/>
+    </row>
+    <row r="1132" spans="3:3">
+      <c r="C1132"/>
+    </row>
+    <row r="1133" spans="3:3">
+      <c r="C1133"/>
+    </row>
+    <row r="1134" spans="3:3">
+      <c r="C1134"/>
+    </row>
+    <row r="1135" spans="3:3">
+      <c r="C1135"/>
+    </row>
+    <row r="1136" spans="3:3">
+      <c r="C1136"/>
+    </row>
+    <row r="1137" spans="3:3">
+      <c r="C1137"/>
+    </row>
+    <row r="1138" spans="3:3">
+      <c r="C1138"/>
+    </row>
+    <row r="1139" spans="3:3">
+      <c r="C1139"/>
+    </row>
+    <row r="1140" spans="3:3">
+      <c r="C1140"/>
+    </row>
+    <row r="1141" spans="3:3">
+      <c r="C1141"/>
+    </row>
+    <row r="1142" spans="3:3">
+      <c r="C1142"/>
+    </row>
+    <row r="1143" spans="3:3">
+      <c r="C1143"/>
+    </row>
+    <row r="1144" spans="3:3">
+      <c r="C1144"/>
+    </row>
+    <row r="1145" spans="3:3">
+      <c r="C1145"/>
+    </row>
+    <row r="1146" spans="3:3">
+      <c r="C1146"/>
+    </row>
+    <row r="1147" spans="3:3">
+      <c r="C1147"/>
+    </row>
+    <row r="1148" spans="3:3">
+      <c r="C1148"/>
+    </row>
+    <row r="1149" spans="3:3">
+      <c r="C1149"/>
+    </row>
+    <row r="1150" spans="3:3">
+      <c r="C1150"/>
+    </row>
+    <row r="1151" spans="3:3">
+      <c r="C1151"/>
+    </row>
+    <row r="1152" spans="3:3">
+      <c r="C1152"/>
+    </row>
+    <row r="1153" spans="3:3">
+      <c r="C1153"/>
+    </row>
+    <row r="1154" spans="3:3">
+      <c r="C1154"/>
+    </row>
+    <row r="1155" spans="3:3">
+      <c r="C1155"/>
+    </row>
+    <row r="1156" spans="3:3">
+      <c r="C1156"/>
+    </row>
+    <row r="1157" spans="3:3">
+      <c r="C1157"/>
+    </row>
+    <row r="1158" spans="3:3">
+      <c r="C1158"/>
+    </row>
+    <row r="1159" spans="3:3">
+      <c r="C1159"/>
+    </row>
+    <row r="1160" spans="3:3">
+      <c r="C1160"/>
+    </row>
+    <row r="1161" spans="3:3">
+      <c r="C1161"/>
+    </row>
+    <row r="1162" spans="3:3">
+      <c r="C1162"/>
+    </row>
+    <row r="1163" spans="3:3">
+      <c r="C1163"/>
+    </row>
+    <row r="1164" spans="3:3">
+      <c r="C1164"/>
+    </row>
+    <row r="1165" spans="3:3">
+      <c r="C1165"/>
+    </row>
+    <row r="1166" spans="3:3">
+      <c r="C1166"/>
+    </row>
+    <row r="1167" spans="3:3">
+      <c r="C1167"/>
+    </row>
+    <row r="1168" spans="3:3">
+      <c r="C1168"/>
+    </row>
+    <row r="1169" spans="3:3">
+      <c r="C1169"/>
+    </row>
+    <row r="1170" spans="3:3">
+      <c r="C1170"/>
+    </row>
+    <row r="1171" spans="3:3">
+      <c r="C1171"/>
+    </row>
+    <row r="1172" spans="3:3">
+      <c r="C1172"/>
+    </row>
+    <row r="1173" spans="3:3">
+      <c r="C1173"/>
+    </row>
+    <row r="1174" spans="3:3">
+      <c r="C1174"/>
+    </row>
+    <row r="1175" spans="3:3">
+      <c r="C1175"/>
+    </row>
+    <row r="1176" spans="3:3">
+      <c r="C1176"/>
+    </row>
+    <row r="1177" spans="3:3">
+      <c r="C1177"/>
+    </row>
+    <row r="1178" spans="3:3">
+      <c r="C1178"/>
+    </row>
+    <row r="1179" spans="3:3">
+      <c r="C1179"/>
+    </row>
+    <row r="1180" spans="3:3">
+      <c r="C1180"/>
+    </row>
+    <row r="1181" spans="3:3">
+      <c r="C1181"/>
+    </row>
+    <row r="1182" spans="3:3">
+      <c r="C1182"/>
+    </row>
+    <row r="1183" spans="3:3">
+      <c r="C1183"/>
+    </row>
+    <row r="1184" spans="3:3">
+      <c r="C1184"/>
+    </row>
+    <row r="1185" spans="3:3">
+      <c r="C1185"/>
+    </row>
+    <row r="1186" spans="3:3">
+      <c r="C1186"/>
+    </row>
+    <row r="1187" spans="3:3">
+      <c r="C1187"/>
+    </row>
+    <row r="1188" spans="3:3">
+      <c r="C1188"/>
+    </row>
+    <row r="1189" spans="3:3">
+      <c r="C1189"/>
+    </row>
+    <row r="1190" spans="3:3">
+      <c r="C1190"/>
+    </row>
+    <row r="1191" spans="3:3">
+      <c r="C1191"/>
+    </row>
+    <row r="1192" spans="3:3">
+      <c r="C1192"/>
+    </row>
+    <row r="1193" spans="3:3">
+      <c r="C1193"/>
+    </row>
+    <row r="1194" spans="3:3">
+      <c r="C1194"/>
+    </row>
+    <row r="1195" spans="3:3">
+      <c r="C1195"/>
+    </row>
+    <row r="1196" spans="3:3">
+      <c r="C1196"/>
+    </row>
+    <row r="1197" spans="3:3">
+      <c r="C1197"/>
+    </row>
+    <row r="1198" spans="3:3">
+      <c r="C1198"/>
+    </row>
+    <row r="1199" spans="3:3">
+      <c r="C1199"/>
+    </row>
+    <row r="1200" spans="3:3">
+      <c r="C1200"/>
+    </row>
+    <row r="1201" spans="3:3">
+      <c r="C1201"/>
+    </row>
+    <row r="1202" spans="3:3">
+      <c r="C1202"/>
+    </row>
+    <row r="1203" spans="3:3">
+      <c r="C1203"/>
+    </row>
+    <row r="1204" spans="3:3">
+      <c r="C1204"/>
+    </row>
+    <row r="1205" spans="3:3">
+      <c r="C1205"/>
+    </row>
+    <row r="1206" spans="3:3">
+      <c r="C1206"/>
+    </row>
+    <row r="1207" spans="3:3">
+      <c r="C1207"/>
+    </row>
+    <row r="1208" spans="3:3">
+      <c r="C1208"/>
+    </row>
+    <row r="1209" spans="3:3">
+      <c r="C1209"/>
+    </row>
+    <row r="1210" spans="3:3">
+      <c r="C1210"/>
+    </row>
+    <row r="1211" spans="3:3">
+      <c r="C1211"/>
+    </row>
+    <row r="1212" spans="3:3">
+      <c r="C1212"/>
+    </row>
+    <row r="1213" spans="3:3">
+      <c r="C1213"/>
+    </row>
+    <row r="1214" spans="3:3">
+      <c r="C1214"/>
+    </row>
+    <row r="1215" spans="3:3">
+      <c r="C1215"/>
+    </row>
+    <row r="1216" spans="3:3">
+      <c r="C1216"/>
+    </row>
+    <row r="1217" spans="3:3">
+      <c r="C1217"/>
+    </row>
+    <row r="1218" spans="3:3">
+      <c r="C1218"/>
+    </row>
+    <row r="1219" spans="3:3">
+      <c r="C1219"/>
+    </row>
+    <row r="1220" spans="3:3">
+      <c r="C1220"/>
+    </row>
+    <row r="1221" spans="3:3">
+      <c r="C1221"/>
+    </row>
+    <row r="1222" spans="3:3">
+      <c r="C1222"/>
+    </row>
+    <row r="1223" spans="3:3">
+      <c r="C1223"/>
+    </row>
+    <row r="1224" spans="3:3">
+      <c r="C1224"/>
+    </row>
+    <row r="1225" spans="3:3">
+      <c r="C1225"/>
+    </row>
+    <row r="1226" spans="3:3">
+      <c r="C1226"/>
+    </row>
+    <row r="1227" spans="3:3">
+      <c r="C1227"/>
+    </row>
+    <row r="1228" spans="3:3">
+      <c r="C1228"/>
+    </row>
+    <row r="1229" spans="3:3">
+      <c r="C1229"/>
+    </row>
+    <row r="1230" spans="3:3">
+      <c r="C1230"/>
+    </row>
+    <row r="1231" spans="3:3">
+      <c r="C1231"/>
+    </row>
+    <row r="1232" spans="3:3">
+      <c r="C1232"/>
+    </row>
+    <row r="1233" spans="3:3">
+      <c r="C1233"/>
+    </row>
+    <row r="1234" spans="3:3">
+      <c r="C1234"/>
+    </row>
+    <row r="1235" spans="3:3">
+      <c r="C1235"/>
+    </row>
+    <row r="1236" spans="3:3">
+      <c r="C1236"/>
+    </row>
+    <row r="1237" spans="3:3">
+      <c r="C1237"/>
+    </row>
+    <row r="1238" spans="3:3">
+      <c r="C1238"/>
+    </row>
+    <row r="1239" spans="3:3">
+      <c r="C1239"/>
+    </row>
+    <row r="1240" spans="3:3">
+      <c r="C1240"/>
+    </row>
+    <row r="1241" spans="3:3">
+      <c r="C1241"/>
+    </row>
+    <row r="1242" spans="3:3">
+      <c r="C1242"/>
+    </row>
+    <row r="1243" spans="3:3">
+      <c r="C1243"/>
+    </row>
+    <row r="1244" spans="3:3">
+      <c r="C1244"/>
+    </row>
+    <row r="1245" spans="3:3">
+      <c r="C1245"/>
+    </row>
+    <row r="1246" spans="3:3">
+      <c r="C1246"/>
+    </row>
+    <row r="1247" spans="3:3">
+      <c r="C1247"/>
+    </row>
+    <row r="1248" spans="3:3">
+      <c r="C1248"/>
+    </row>
+    <row r="1249" spans="3:3">
+      <c r="C1249"/>
+    </row>
+    <row r="1250" spans="3:3">
+      <c r="C1250"/>
+    </row>
+    <row r="1251" spans="3:3">
+      <c r="C1251"/>
+    </row>
+    <row r="1252" spans="3:3">
+      <c r="C1252"/>
+    </row>
+    <row r="1253" spans="3:3">
+      <c r="C1253"/>
+    </row>
+    <row r="1254" spans="3:3">
+      <c r="C1254"/>
+    </row>
+    <row r="1255" spans="3:3">
+      <c r="C1255"/>
+    </row>
+    <row r="1256" spans="3:3">
+      <c r="C1256"/>
+    </row>
+    <row r="1257" spans="3:3">
+      <c r="C1257"/>
+    </row>
+    <row r="1258" spans="3:3">
+      <c r="C1258"/>
+    </row>
+    <row r="1259" spans="3:3">
+      <c r="C1259"/>
+    </row>
+    <row r="1260" spans="3:3">
+      <c r="C1260"/>
+    </row>
+    <row r="1261" spans="3:3">
+      <c r="C1261"/>
+    </row>
+    <row r="1262" spans="3:3">
+      <c r="C1262"/>
+    </row>
+    <row r="1263" spans="3:3">
+      <c r="C1263"/>
+    </row>
+    <row r="1264" spans="3:3">
+      <c r="C1264"/>
+    </row>
+    <row r="1265" spans="3:3">
+      <c r="C1265"/>
+    </row>
+    <row r="1266" spans="3:3">
+      <c r="C1266"/>
+    </row>
+    <row r="1267" spans="3:3">
+      <c r="C1267"/>
+    </row>
+    <row r="1268" spans="3:3">
+      <c r="C1268"/>
+    </row>
+    <row r="1269" spans="3:3">
+      <c r="C1269"/>
+    </row>
+    <row r="1270" spans="3:3">
+      <c r="C1270"/>
+    </row>
+    <row r="1271" spans="3:3">
+      <c r="C1271"/>
+    </row>
+    <row r="1272" spans="3:3">
+      <c r="C1272"/>
+    </row>
+    <row r="1273" spans="3:3">
+      <c r="C1273"/>
+    </row>
+    <row r="1274" spans="3:3">
+      <c r="C1274"/>
+    </row>
+    <row r="1275" spans="3:3">
+      <c r="C1275"/>
+    </row>
+    <row r="1276" spans="3:3">
+      <c r="C1276"/>
+    </row>
+    <row r="1277" spans="3:3">
+      <c r="C1277"/>
+    </row>
+    <row r="1278" spans="3:3">
+      <c r="C1278"/>
+    </row>
+    <row r="1279" spans="3:3">
+      <c r="C1279"/>
+    </row>
+    <row r="1280" spans="3:3">
+      <c r="C1280"/>
+    </row>
+    <row r="1281" spans="3:3">
+      <c r="C1281"/>
+    </row>
+    <row r="1282" spans="3:3">
+      <c r="C1282"/>
+    </row>
+    <row r="1283" spans="3:3">
+      <c r="C1283"/>
+    </row>
+    <row r="1284" spans="3:3">
+      <c r="C1284"/>
+    </row>
+    <row r="1285" spans="3:3">
+      <c r="C1285"/>
+    </row>
+    <row r="1286" spans="3:3">
+      <c r="C1286"/>
+    </row>
+    <row r="1287" spans="3:3">
+      <c r="C1287"/>
+    </row>
+    <row r="1288" spans="3:3">
+      <c r="C1288"/>
+    </row>
+    <row r="1289" spans="3:3">
+      <c r="C1289"/>
+    </row>
+    <row r="1290" spans="3:3">
+      <c r="C1290"/>
+    </row>
+    <row r="1291" spans="3:3">
+      <c r="C1291"/>
+    </row>
+    <row r="1292" spans="3:3">
+      <c r="C1292"/>
+    </row>
+    <row r="1293" spans="3:3">
+      <c r="C1293"/>
+    </row>
+    <row r="1294" spans="3:3">
+      <c r="C1294"/>
+    </row>
+    <row r="1295" spans="3:3">
+      <c r="C1295"/>
+    </row>
+    <row r="1296" spans="3:3">
+      <c r="C1296"/>
+    </row>
+    <row r="1297" spans="3:3">
+      <c r="C1297"/>
+    </row>
+    <row r="1298" spans="3:3">
+      <c r="C1298"/>
+    </row>
+    <row r="1299" spans="3:3">
+      <c r="C1299"/>
+    </row>
+    <row r="1300" spans="3:3">
+      <c r="C1300"/>
+    </row>
+    <row r="1301" spans="3:3">
+      <c r="C1301"/>
+    </row>
+    <row r="1302" spans="3:3">
+      <c r="C1302"/>
+    </row>
+    <row r="1303" spans="3:3">
+      <c r="C1303"/>
+    </row>
+    <row r="1304" spans="3:3">
+      <c r="C1304"/>
+    </row>
+    <row r="1305" spans="3:3">
+      <c r="C1305"/>
+    </row>
+    <row r="1306" spans="3:3">
+      <c r="C1306"/>
+    </row>
+    <row r="1307" spans="3:3">
+      <c r="C1307"/>
+    </row>
+    <row r="1308" spans="3:3">
+      <c r="C1308"/>
+    </row>
+    <row r="1309" spans="3:3">
+      <c r="C1309"/>
+    </row>
+    <row r="1310" spans="3:3">
+      <c r="C1310"/>
+    </row>
+    <row r="1311" spans="3:3">
+      <c r="C1311"/>
+    </row>
+    <row r="1312" spans="3:3">
+      <c r="C1312"/>
+    </row>
+    <row r="1313" spans="3:3">
+      <c r="C1313"/>
+    </row>
+    <row r="1314" spans="3:3">
+      <c r="C1314"/>
+    </row>
+    <row r="1315" spans="3:3">
+      <c r="C1315"/>
+    </row>
+    <row r="1316" spans="3:3">
+      <c r="C1316"/>
+    </row>
+    <row r="1317" spans="3:3">
+      <c r="C1317"/>
+    </row>
+    <row r="1318" spans="3:3">
+      <c r="C1318"/>
+    </row>
+    <row r="1319" spans="3:3">
+      <c r="C1319"/>
+    </row>
+    <row r="1320" spans="3:3">
+      <c r="C1320"/>
+    </row>
+    <row r="1321" spans="3:3">
+      <c r="C1321"/>
+    </row>
+    <row r="1322" spans="3:3">
+      <c r="C1322"/>
+    </row>
+    <row r="1323" spans="3:3">
+      <c r="C1323"/>
+    </row>
+    <row r="1324" spans="3:3">
+      <c r="C1324"/>
+    </row>
+    <row r="1325" spans="3:3">
+      <c r="C1325"/>
+    </row>
+    <row r="1326" spans="3:3">
+      <c r="C1326"/>
+    </row>
+    <row r="1327" spans="3:3">
+      <c r="C1327"/>
+    </row>
+    <row r="1328" spans="3:3">
+      <c r="C1328"/>
+    </row>
+    <row r="1329" spans="3:3">
+      <c r="C1329"/>
+    </row>
+    <row r="1330" spans="3:3">
+      <c r="C1330"/>
+    </row>
+    <row r="1331" spans="3:3">
+      <c r="C1331"/>
+    </row>
+    <row r="1332" spans="3:3">
+      <c r="C1332"/>
+    </row>
+    <row r="1333" spans="3:3">
+      <c r="C1333"/>
+    </row>
+    <row r="1334" spans="3:3">
+      <c r="C1334"/>
+    </row>
+    <row r="1335" spans="3:3">
+      <c r="C1335"/>
+    </row>
+    <row r="1336" spans="3:3">
+      <c r="C1336"/>
+    </row>
+    <row r="1337" spans="3:3">
+      <c r="C1337"/>
+    </row>
+    <row r="1338" spans="3:3">
+      <c r="C1338"/>
+    </row>
+    <row r="1339" spans="3:3">
+      <c r="C1339"/>
+    </row>
+    <row r="1340" spans="3:3">
+      <c r="C1340"/>
+    </row>
+    <row r="1341" spans="3:3">
+      <c r="C1341"/>
+    </row>
+    <row r="1342" spans="3:3">
+      <c r="C1342"/>
+    </row>
+    <row r="1343" spans="3:3">
+      <c r="C1343"/>
+    </row>
+    <row r="1344" spans="3:3">
+      <c r="C1344"/>
+    </row>
+    <row r="1345" spans="3:3">
+      <c r="C1345"/>
+    </row>
+    <row r="1346" spans="3:3">
+      <c r="C1346"/>
+    </row>
+    <row r="1347" spans="3:3">
+      <c r="C1347"/>
+    </row>
+    <row r="1348" spans="3:3">
+      <c r="C1348"/>
+    </row>
+    <row r="1349" spans="3:3">
+      <c r="C1349"/>
+    </row>
+    <row r="1350" spans="3:3">
+      <c r="C1350"/>
+    </row>
+    <row r="1351" spans="3:3">
+      <c r="C1351"/>
+    </row>
+    <row r="1352" spans="3:3">
+      <c r="C1352"/>
+    </row>
+    <row r="1353" spans="3:3">
+      <c r="C1353"/>
+    </row>
+    <row r="1354" spans="3:3">
+      <c r="C1354"/>
+    </row>
+    <row r="1355" spans="3:3">
+      <c r="C1355"/>
+    </row>
+    <row r="1356" spans="3:3">
+      <c r="C1356"/>
+    </row>
+    <row r="1357" spans="3:3">
+      <c r="C1357"/>
+    </row>
+    <row r="1358" spans="3:3">
+      <c r="C1358"/>
+    </row>
+    <row r="1359" spans="3:3">
+      <c r="C1359"/>
+    </row>
+    <row r="1360" spans="3:3">
+      <c r="C1360"/>
+    </row>
+    <row r="1361" spans="3:3">
+      <c r="C1361"/>
+    </row>
+    <row r="1362" spans="3:3">
+      <c r="C1362"/>
+    </row>
+    <row r="1363" spans="3:3">
+      <c r="C1363"/>
+    </row>
+    <row r="1364" spans="3:3">
+      <c r="C1364"/>
+    </row>
+    <row r="1365" spans="3:3">
+      <c r="C1365"/>
+    </row>
+    <row r="1366" spans="3:3">
+      <c r="C1366"/>
+    </row>
+    <row r="1367" spans="3:3">
+      <c r="C1367"/>
+    </row>
+    <row r="1368" spans="3:3">
+      <c r="C1368"/>
+    </row>
+    <row r="1369" spans="3:3">
+      <c r="C1369"/>
+    </row>
+    <row r="1370" spans="3:3">
+      <c r="C1370"/>
+    </row>
+    <row r="1371" spans="3:3">
+      <c r="C1371"/>
+    </row>
+    <row r="1372" spans="3:3">
+      <c r="C1372"/>
+    </row>
+    <row r="1373" spans="3:3">
+      <c r="C1373"/>
+    </row>
+    <row r="1374" spans="3:3">
+      <c r="C1374"/>
+    </row>
+    <row r="1375" spans="3:3">
+      <c r="C1375"/>
+    </row>
+    <row r="1376" spans="3:3">
+      <c r="C1376"/>
+    </row>
+    <row r="1377" spans="3:3">
+      <c r="C1377"/>
+    </row>
+    <row r="1378" spans="3:3">
+      <c r="C1378"/>
+    </row>
+    <row r="1379" spans="3:3">
+      <c r="C1379"/>
+    </row>
+    <row r="1380" spans="3:3">
+      <c r="C1380"/>
+    </row>
+    <row r="1381" spans="3:3">
+      <c r="C1381"/>
+    </row>
+    <row r="1382" spans="3:3">
+      <c r="C1382"/>
+    </row>
+    <row r="1383" spans="3:3">
+      <c r="C1383"/>
+    </row>
+    <row r="1384" spans="3:3">
+      <c r="C1384"/>
+    </row>
+    <row r="1385" spans="3:3">
+      <c r="C1385"/>
+    </row>
+    <row r="1386" spans="3:3">
+      <c r="C1386"/>
+    </row>
+    <row r="1387" spans="3:3">
+      <c r="C1387"/>
+    </row>
+    <row r="1388" spans="3:3">
+      <c r="C1388"/>
+    </row>
+    <row r="1389" spans="3:3">
+      <c r="C1389"/>
+    </row>
+    <row r="1390" spans="3:3">
+      <c r="C1390"/>
+    </row>
+    <row r="1391" spans="3:3">
+      <c r="C1391"/>
+    </row>
+    <row r="1392" spans="3:3">
+      <c r="C1392"/>
+    </row>
+    <row r="1393" spans="3:3">
+      <c r="C1393"/>
+    </row>
+    <row r="1394" spans="3:3">
+      <c r="C1394"/>
+    </row>
+    <row r="1395" spans="3:3">
+      <c r="C1395"/>
+    </row>
+    <row r="1396" spans="3:3">
+      <c r="C1396"/>
+    </row>
+    <row r="1397" spans="3:3">
+      <c r="C1397"/>
+    </row>
+    <row r="1398" spans="3:3">
+      <c r="C1398"/>
+    </row>
+    <row r="1399" spans="3:3">
+      <c r="C1399"/>
+    </row>
+    <row r="1400" spans="3:3">
+      <c r="C1400"/>
+    </row>
+    <row r="1401" spans="3:3">
+      <c r="C1401"/>
+    </row>
+    <row r="1402" spans="3:3">
+      <c r="C1402"/>
+    </row>
+    <row r="1403" spans="3:3">
+      <c r="C1403"/>
+    </row>
+    <row r="1404" spans="3:3">
+      <c r="C1404"/>
+    </row>
+    <row r="1405" spans="3:3">
+      <c r="C1405"/>
+    </row>
+    <row r="1406" spans="3:3">
+      <c r="C1406"/>
+    </row>
+    <row r="1407" spans="3:3">
+      <c r="C1407"/>
+    </row>
+    <row r="1408" spans="3:3">
+      <c r="C1408"/>
+    </row>
+    <row r="1409" spans="3:3">
+      <c r="C1409"/>
+    </row>
+    <row r="1410" spans="3:3">
+      <c r="C1410"/>
+    </row>
+    <row r="1411" spans="3:3">
+      <c r="C1411"/>
+    </row>
+    <row r="1412" spans="3:3">
+      <c r="C1412"/>
+    </row>
+    <row r="1413" spans="3:3">
+      <c r="C1413"/>
+    </row>
+    <row r="1414" spans="3:3">
+      <c r="C1414"/>
+    </row>
+    <row r="1415" spans="3:3">
+      <c r="C1415"/>
+    </row>
+    <row r="1416" spans="3:3">
+      <c r="C1416"/>
+    </row>
+    <row r="1417" spans="3:3">
+      <c r="C1417"/>
+    </row>
+    <row r="1418" spans="3:3">
+      <c r="C1418"/>
+    </row>
+    <row r="1419" spans="3:3">
+      <c r="C1419"/>
+    </row>
+    <row r="1420" spans="3:3">
+      <c r="C1420"/>
+    </row>
+    <row r="1421" spans="3:3">
+      <c r="C1421"/>
+    </row>
+    <row r="1422" spans="3:3">
+      <c r="C1422"/>
+    </row>
+    <row r="1423" spans="3:3">
+      <c r="C1423"/>
+    </row>
+    <row r="1424" spans="3:3">
+      <c r="C1424"/>
+    </row>
+    <row r="1425" spans="3:3">
+      <c r="C1425"/>
+    </row>
+    <row r="1426" spans="3:3">
+      <c r="C1426"/>
+    </row>
+    <row r="1427" spans="3:3">
+      <c r="C1427"/>
+    </row>
+    <row r="1428" spans="3:3">
+      <c r="C1428"/>
+    </row>
+    <row r="1429" spans="3:3">
+      <c r="C1429"/>
+    </row>
+    <row r="1430" spans="3:3">
+      <c r="C1430"/>
+    </row>
+    <row r="1431" spans="3:3">
+      <c r="C1431"/>
+    </row>
+    <row r="1432" spans="3:3">
+      <c r="C1432"/>
+    </row>
+    <row r="1433" spans="3:3">
+      <c r="C1433"/>
+    </row>
+    <row r="1434" spans="3:3">
+      <c r="C1434"/>
+    </row>
+    <row r="1435" spans="3:3">
+      <c r="C1435"/>
+    </row>
+    <row r="1436" spans="3:3">
+      <c r="C1436"/>
+    </row>
+    <row r="1437" spans="3:3">
+      <c r="C1437"/>
+    </row>
+    <row r="1438" spans="3:3">
+      <c r="C1438"/>
+    </row>
+    <row r="1439" spans="3:3">
+      <c r="C1439"/>
+    </row>
+    <row r="1440" spans="3:3">
+      <c r="C1440"/>
+    </row>
+    <row r="1441" spans="3:3">
+      <c r="C1441"/>
+    </row>
+    <row r="1442" spans="3:3">
+      <c r="C1442"/>
+    </row>
+    <row r="1443" spans="3:3">
+      <c r="C1443"/>
+    </row>
+    <row r="1444" spans="3:3">
+      <c r="C1444"/>
+    </row>
+    <row r="1445" spans="3:3">
+      <c r="C1445"/>
+    </row>
+    <row r="1446" spans="3:3">
+      <c r="C1446"/>
+    </row>
+    <row r="1447" spans="3:3">
+      <c r="C1447"/>
+    </row>
+    <row r="1448" spans="3:3">
+      <c r="C1448"/>
+    </row>
+    <row r="1449" spans="3:3">
+      <c r="C1449"/>
+    </row>
+    <row r="1450" spans="3:3">
+      <c r="C1450"/>
+    </row>
+    <row r="1451" spans="3:3">
+      <c r="C1451"/>
+    </row>
+    <row r="1452" spans="3:3">
+      <c r="C1452"/>
+    </row>
+    <row r="1453" spans="3:3">
+      <c r="C1453"/>
+    </row>
+    <row r="1454" spans="3:3">
+      <c r="C1454"/>
+    </row>
+    <row r="1455" spans="3:3">
+      <c r="C1455"/>
+    </row>
+    <row r="1456" spans="3:3">
+      <c r="C1456"/>
+    </row>
+    <row r="1457" spans="3:3">
+      <c r="C1457"/>
+    </row>
+    <row r="1458" spans="3:3">
+      <c r="C1458"/>
+    </row>
+    <row r="1459" spans="3:3">
+      <c r="C1459"/>
+    </row>
+    <row r="1460" spans="3:3">
+      <c r="C1460"/>
+    </row>
+    <row r="1461" spans="3:3">
+      <c r="C1461"/>
+    </row>
+    <row r="1462" spans="3:3">
+      <c r="C1462"/>
+    </row>
+    <row r="1463" spans="3:3">
+      <c r="C1463"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="10" spans="5:5">
+      <c r="E10" s="17"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>